<commit_message>
saving compiled final data
</commit_message>
<xml_diff>
--- a/1-Data-Codes/2-Final_Data/deficits_allyears.xlsx
+++ b/1-Data-Codes/2-Final_Data/deficits_allyears.xlsx
@@ -380,28 +380,28 @@
         <v>1</v>
       </c>
       <c r="B2" s="0">
-        <v>-12611.341878890991</v>
+        <v>-10873.127998352051</v>
       </c>
       <c r="C2" s="0">
-        <v>-13426.571701049805</v>
+        <v>-11708.108806610107</v>
       </c>
       <c r="D2" s="0">
-        <v>-13014.954107284546</v>
+        <v>-11450.99732208252</v>
       </c>
       <c r="E2" s="0">
-        <v>-14090.888679504395</v>
+        <v>-12045.834182739258</v>
       </c>
       <c r="F2" s="0">
-        <v>-14924.809882640839</v>
+        <v>-12661.801446914673</v>
       </c>
       <c r="G2" s="0">
-        <v>-19137.045877456665</v>
+        <v>-16822.091156005859</v>
       </c>
       <c r="H2" s="0">
-        <v>-16476.866760253906</v>
+        <v>-14246.990020751953</v>
       </c>
       <c r="I2" s="0">
-        <v>-17222.96501159668</v>
+        <v>-14903.640640258789</v>
       </c>
     </row>
     <row r="3">
@@ -409,28 +409,28 @@
         <v>2</v>
       </c>
       <c r="B3" s="0">
-        <v>-1608.1422824859619</v>
+        <v>-925.74407005310059</v>
       </c>
       <c r="C3" s="0">
-        <v>-900.684250831604</v>
+        <v>-293.51819610595703</v>
       </c>
       <c r="D3" s="0">
-        <v>-2686.3729286193848</v>
+        <v>-2198.5029821395874</v>
       </c>
       <c r="E3" s="0">
-        <v>-2809.1413488388062</v>
+        <v>-2084.0344944000244</v>
       </c>
       <c r="F3" s="0">
-        <v>-3244.5525236129761</v>
+        <v>-2635.4618587493896</v>
       </c>
       <c r="G3" s="0">
-        <v>-4308.2430956959724</v>
+        <v>-4676.6120461821556</v>
       </c>
       <c r="H3" s="0">
-        <v>-5209.147292137146</v>
+        <v>-5476.8604717254639</v>
       </c>
       <c r="I3" s="0">
-        <v>-4614.4413642883301</v>
+        <v>-4878.2054758071899</v>
       </c>
     </row>
     <row r="4">
@@ -438,28 +438,28 @@
         <v>3</v>
       </c>
       <c r="B4" s="0">
-        <v>-4935.1403198242187</v>
+        <v>-2601.8461608886719</v>
       </c>
       <c r="C4" s="0">
-        <v>-4686.9011993408203</v>
+        <v>-2393.731201171875</v>
       </c>
       <c r="D4" s="0">
-        <v>-6531.7808380126953</v>
+        <v>-4283.9151611328125</v>
       </c>
       <c r="E4" s="0">
-        <v>-3162.4334716796875</v>
+        <v>-624.95346069335937</v>
       </c>
       <c r="F4" s="0">
-        <v>849.28775024414062</v>
+        <v>4114.259033203125</v>
       </c>
       <c r="G4" s="0">
-        <v>2545.8428802490234</v>
+        <v>6347.6596069335937</v>
       </c>
       <c r="H4" s="0">
-        <v>9239.3572082519531</v>
+        <v>13334.445337295532</v>
       </c>
       <c r="I4" s="0">
-        <v>8809.0408630371094</v>
+        <v>13378.335960388184</v>
       </c>
     </row>
     <row r="5">
@@ -467,28 +467,28 @@
         <v>4</v>
       </c>
       <c r="B5" s="0">
-        <v>1524.578052520752</v>
+        <v>1068.0323944091797</v>
       </c>
       <c r="C5" s="0">
-        <v>-13.966897964477539</v>
+        <v>-492.30663299560547</v>
       </c>
       <c r="D5" s="0">
-        <v>236.51803970336914</v>
+        <v>-207.75915145874023</v>
       </c>
       <c r="E5" s="0">
-        <v>688.81691741943359</v>
+        <v>141.83448791503906</v>
       </c>
       <c r="F5" s="0">
-        <v>114.84868621826172</v>
+        <v>-451.23518371582031</v>
       </c>
       <c r="G5" s="0">
-        <v>-5470.5318412780762</v>
+        <v>-6527.8411445617676</v>
       </c>
       <c r="H5" s="0">
-        <v>-7838.3638076782227</v>
+        <v>-8963.4467010498047</v>
       </c>
       <c r="I5" s="0">
-        <v>-7418.9776000976562</v>
+        <v>-8738.7780876159668</v>
       </c>
     </row>
     <row r="6">
@@ -496,28 +496,28 @@
         <v>5</v>
       </c>
       <c r="B6" s="0">
-        <v>-35604.377212524414</v>
+        <v>-38984.251098632813</v>
       </c>
       <c r="C6" s="0">
-        <v>-39066.264373779297</v>
+        <v>-43136.914672851563</v>
       </c>
       <c r="D6" s="0">
-        <v>-28999.640106201172</v>
+        <v>-31908.666931152344</v>
       </c>
       <c r="E6" s="0">
-        <v>-5759.8784790039062</v>
+        <v>-10767.0830078125</v>
       </c>
       <c r="F6" s="0">
-        <v>503.281982421875</v>
+        <v>-3187.275146484375</v>
       </c>
       <c r="G6" s="0">
-        <v>14405.457153320313</v>
+        <v>18280.338714599609</v>
       </c>
       <c r="H6" s="0">
-        <v>22133.752563476563</v>
+        <v>24794.915893554688</v>
       </c>
       <c r="I6" s="0">
-        <v>-13109.521362304687</v>
+        <v>-10094.875</v>
       </c>
     </row>
     <row r="7">
@@ -525,28 +525,28 @@
         <v>6</v>
       </c>
       <c r="B7" s="0">
-        <v>19465.166687011719</v>
+        <v>20309.761192321777</v>
       </c>
       <c r="C7" s="0">
-        <v>17525.912117004395</v>
+        <v>18373.537939071655</v>
       </c>
       <c r="D7" s="0">
-        <v>12251.887916564941</v>
+        <v>13070.995079040527</v>
       </c>
       <c r="E7" s="0">
-        <v>8375.5609512329102</v>
+        <v>9299.0497894287109</v>
       </c>
       <c r="F7" s="0">
-        <v>-600.74692535400391</v>
+        <v>-1432.8338918685913</v>
       </c>
       <c r="G7" s="0">
-        <v>-788.64837646484375</v>
+        <v>-4874.4433441162109</v>
       </c>
       <c r="H7" s="0">
-        <v>-3378.4465026855469</v>
+        <v>-5124.8142395019531</v>
       </c>
       <c r="I7" s="0">
-        <v>3936.7264709472656</v>
+        <v>-384.6815185546875</v>
       </c>
     </row>
     <row r="8">
@@ -554,28 +554,28 @@
         <v>7</v>
       </c>
       <c r="B8" s="0">
-        <v>23788.470916748047</v>
+        <v>19823.726894378662</v>
       </c>
       <c r="C8" s="0">
-        <v>25039.650493621826</v>
+        <v>21346.617713928223</v>
       </c>
       <c r="D8" s="0">
-        <v>17082.077011108398</v>
+        <v>18062.803039550781</v>
       </c>
       <c r="E8" s="0">
-        <v>15865.149169921875</v>
+        <v>12622.651321411133</v>
       </c>
       <c r="F8" s="0">
-        <v>19058.704467773438</v>
+        <v>1699.5364685058594</v>
       </c>
       <c r="G8" s="0">
-        <v>14439.106932163239</v>
+        <v>7410.0629518032074</v>
       </c>
       <c r="H8" s="0">
-        <v>13318.838356018066</v>
+        <v>7519.4964141845703</v>
       </c>
       <c r="I8" s="0">
-        <v>23774.811340332031</v>
+        <v>24483.235061645508</v>
       </c>
     </row>
     <row r="9">
@@ -583,28 +583,28 @@
         <v>8</v>
       </c>
       <c r="B9" s="0">
-        <v>21133.187590479851</v>
+        <v>22220.653880357742</v>
       </c>
       <c r="C9" s="0">
-        <v>23314.16773223877</v>
+        <v>24431.200061798096</v>
       </c>
       <c r="D9" s="0">
-        <v>20764.716090679169</v>
+        <v>21872.942145347595</v>
       </c>
       <c r="E9" s="0">
-        <v>20591.906446456909</v>
+        <v>21824.908760070801</v>
       </c>
       <c r="F9" s="0">
-        <v>20648.441822052002</v>
+        <v>21735.130888938904</v>
       </c>
       <c r="G9" s="0">
-        <v>15656.974853515625</v>
+        <v>16635.238922119141</v>
       </c>
       <c r="H9" s="0">
-        <v>16593.656410217285</v>
+        <v>14189.734565734863</v>
       </c>
       <c r="I9" s="0">
-        <v>14103.333111763</v>
+        <v>9214.5211849212646</v>
       </c>
     </row>
     <row r="10">
@@ -612,28 +612,28 @@
         <v>9</v>
       </c>
       <c r="B10" s="0">
-        <v>-71034.528076171875</v>
+        <v>-70934.971862792969</v>
       </c>
       <c r="C10" s="0">
-        <v>-60300.84814453125</v>
+        <v>-60296.177978515625</v>
       </c>
       <c r="D10" s="0">
-        <v>-43669.6552734375</v>
+        <v>-43532.788940429688</v>
       </c>
       <c r="E10" s="0">
-        <v>-34761.750732421875</v>
+        <v>-34654.93701171875</v>
       </c>
       <c r="F10" s="0">
-        <v>-29417.88818359375</v>
+        <v>-28901.034484863281</v>
       </c>
       <c r="G10" s="0">
-        <v>-11484.636474609375</v>
+        <v>-8143.5535278320312</v>
       </c>
       <c r="H10" s="0">
-        <v>-16807.317138671875</v>
+        <v>-13658.361328125</v>
       </c>
       <c r="I10" s="0">
-        <v>-43660.07861328125</v>
+        <v>-39654.66552734375</v>
       </c>
     </row>
     <row r="11">
@@ -641,28 +641,28 @@
         <v>10</v>
       </c>
       <c r="B11" s="0">
-        <v>46376.1201171875</v>
+        <v>47704.217185974121</v>
       </c>
       <c r="C11" s="0">
-        <v>45334.921081542969</v>
+        <v>46442.598796844482</v>
       </c>
       <c r="D11" s="0">
-        <v>38657.700439453125</v>
+        <v>39671.228057861328</v>
       </c>
       <c r="E11" s="0">
-        <v>39904.538177490234</v>
+        <v>40937.727310180664</v>
       </c>
       <c r="F11" s="0">
-        <v>45081.318176269531</v>
+        <v>46355.563674926758</v>
       </c>
       <c r="G11" s="0">
-        <v>41318.212219238281</v>
+        <v>42098.249389648438</v>
       </c>
       <c r="H11" s="0">
-        <v>34339.515075683594</v>
+        <v>35797.918975830078</v>
       </c>
       <c r="I11" s="0">
-        <v>27692.263275146484</v>
+        <v>30183.326782226563</v>
       </c>
     </row>
     <row r="12">
@@ -670,28 +670,28 @@
         <v>11</v>
       </c>
       <c r="B12" s="0">
-        <v>-3198.1759519577026</v>
+        <v>-3991.8445873260498</v>
       </c>
       <c r="C12" s="0">
-        <v>-2820.4071815013885</v>
+        <v>-3531.4633331298828</v>
       </c>
       <c r="D12" s="0">
-        <v>-1843.2972927093506</v>
+        <v>-2298.766529083252</v>
       </c>
       <c r="E12" s="0">
-        <v>-1204.4396362304687</v>
+        <v>-1653.7069931030273</v>
       </c>
       <c r="F12" s="0">
-        <v>918.20102691650391</v>
+        <v>264.6221923828125</v>
       </c>
       <c r="G12" s="0">
-        <v>131.57121658325195</v>
+        <v>-302.2756462097168</v>
       </c>
       <c r="H12" s="0">
-        <v>-827.17090606689453</v>
+        <v>-1319.3425064086914</v>
       </c>
       <c r="I12" s="0">
-        <v>-1123.4336242675781</v>
+        <v>-1701.9941787719727</v>
       </c>
     </row>
     <row r="13">
@@ -699,28 +699,28 @@
         <v>12</v>
       </c>
       <c r="B13" s="0">
-        <v>930.86605930328369</v>
+        <v>-3572.7366619110107</v>
       </c>
       <c r="C13" s="0">
-        <v>1364.0006370544434</v>
+        <v>-3296.7632646560669</v>
       </c>
       <c r="D13" s="0">
-        <v>557.73124217987061</v>
+        <v>-3812.9227828979492</v>
       </c>
       <c r="E13" s="0">
-        <v>1320.0049123764038</v>
+        <v>-3847.6047210693359</v>
       </c>
       <c r="F13" s="0">
-        <v>1878.442850112915</v>
+        <v>-4135.4429569244385</v>
       </c>
       <c r="G13" s="0">
-        <v>-2353.958251953125</v>
+        <v>-5804.0412750244141</v>
       </c>
       <c r="H13" s="0">
-        <v>132.18974304199219</v>
+        <v>-3585.3817749023437</v>
       </c>
       <c r="I13" s="0">
-        <v>2024.1250610351563</v>
+        <v>-2174.2610168457031</v>
       </c>
     </row>
     <row r="14">
@@ -728,28 +728,28 @@
         <v>13</v>
       </c>
       <c r="B14" s="0">
-        <v>-2958.8227844238281</v>
+        <v>-7480.7774047851562</v>
       </c>
       <c r="C14" s="0">
-        <v>-1197.6940002441406</v>
+        <v>-6005.9500122070312</v>
       </c>
       <c r="D14" s="0">
-        <v>-2566.7352600097656</v>
+        <v>-6671.3290100097656</v>
       </c>
       <c r="E14" s="0">
-        <v>-13094.760437011719</v>
+        <v>-19321.469055175781</v>
       </c>
       <c r="F14" s="0">
-        <v>-19824.046569824219</v>
+        <v>-27386.585693359375</v>
       </c>
       <c r="G14" s="0">
-        <v>-14114.899200439453</v>
+        <v>-17283.932037353516</v>
       </c>
       <c r="H14" s="0">
-        <v>562.18844604492187</v>
+        <v>-2795.3884887695312</v>
       </c>
       <c r="I14" s="0">
-        <v>11965.893737792969</v>
+        <v>9005.1469116210937</v>
       </c>
     </row>
     <row r="15">
@@ -757,28 +757,28 @@
         <v>14</v>
       </c>
       <c r="B15" s="0">
-        <v>3931.72492839396</v>
+        <v>2138.4760798215866</v>
       </c>
       <c r="C15" s="0">
-        <v>-1216.2500195503235</v>
+        <v>-3068.2301774024963</v>
       </c>
       <c r="D15" s="0">
-        <v>-7336.7512550354004</v>
+        <v>-8998.7890586853027</v>
       </c>
       <c r="E15" s="0">
-        <v>-6460.1561584472656</v>
+        <v>-8461.9663772583008</v>
       </c>
       <c r="F15" s="0">
-        <v>-12882.211067199707</v>
+        <v>-15681.342658996582</v>
       </c>
       <c r="G15" s="0">
-        <v>-17860.494612693787</v>
+        <v>-24925.209503173828</v>
       </c>
       <c r="H15" s="0">
-        <v>-19254.617269515991</v>
+        <v>-26847.240951538086</v>
       </c>
       <c r="I15" s="0">
-        <v>-15555.972612380981</v>
+        <v>-23990.977146148682</v>
       </c>
     </row>
     <row r="16">
@@ -786,28 +786,28 @@
         <v>15</v>
       </c>
       <c r="B16" s="0">
-        <v>5842.6679992675781</v>
+        <v>1438.5492973327637</v>
       </c>
       <c r="C16" s="0">
-        <v>3953.4971618652344</v>
+        <v>-610.52996826171875</v>
       </c>
       <c r="D16" s="0">
-        <v>4058.6273193359375</v>
+        <v>-167.62702178955078</v>
       </c>
       <c r="E16" s="0">
-        <v>8333.0724105834961</v>
+        <v>3326.400318145752</v>
       </c>
       <c r="F16" s="0">
-        <v>12932.575782775879</v>
+        <v>7174.2282638549805</v>
       </c>
       <c r="G16" s="0">
-        <v>11642.917127609253</v>
+        <v>6894.0826807022095</v>
       </c>
       <c r="H16" s="0">
-        <v>9426.6464557647705</v>
+        <v>4390.4054355621338</v>
       </c>
       <c r="I16" s="0">
-        <v>19736.617765426636</v>
+        <v>13774.169589519501</v>
       </c>
     </row>
     <row r="17">
@@ -815,28 +815,28 @@
         <v>16</v>
       </c>
       <c r="B17" s="0">
-        <v>3361.9060325622559</v>
+        <v>2723.4785995483398</v>
       </c>
       <c r="C17" s="0">
-        <v>2180.9193878173828</v>
+        <v>1550.3070983886719</v>
       </c>
       <c r="D17" s="0">
-        <v>2347.6820106506348</v>
+        <v>1717.5371475219727</v>
       </c>
       <c r="E17" s="0">
-        <v>1046.0266990661621</v>
+        <v>300.99237060546875</v>
       </c>
       <c r="F17" s="0">
-        <v>-3500.3955078125</v>
+        <v>-4170.3481750488281</v>
       </c>
       <c r="G17" s="0">
-        <v>-4490.2590289115906</v>
+        <v>-6924.8609910011292</v>
       </c>
       <c r="H17" s="0">
-        <v>-2399.2226219177246</v>
+        <v>-5073.3579292297363</v>
       </c>
       <c r="I17" s="0">
-        <v>2034.4052686691284</v>
+        <v>-1184.0953326225281</v>
       </c>
     </row>
     <row r="18">
@@ -844,28 +844,28 @@
         <v>17</v>
       </c>
       <c r="B18" s="0">
-        <v>-23617.238677978516</v>
+        <v>-23364.464416503906</v>
       </c>
       <c r="C18" s="0">
-        <v>-23246.869979858398</v>
+        <v>-23149.589813232422</v>
       </c>
       <c r="D18" s="0">
-        <v>-24021.346649169922</v>
+        <v>-23896.423194885254</v>
       </c>
       <c r="E18" s="0">
-        <v>-25731.313766479492</v>
+        <v>-25493.244598388672</v>
       </c>
       <c r="F18" s="0">
-        <v>-27202.454803466797</v>
+        <v>-27204.308303833008</v>
       </c>
       <c r="G18" s="0">
-        <v>-28165.816734313965</v>
+        <v>-28268.646301269531</v>
       </c>
       <c r="H18" s="0">
-        <v>-30528.183120727539</v>
+        <v>-30034.901847839355</v>
       </c>
       <c r="I18" s="0">
-        <v>-28512.712749481201</v>
+        <v>-29284.452857971191</v>
       </c>
     </row>
     <row r="19">
@@ -873,28 +873,28 @@
         <v>18</v>
       </c>
       <c r="B19" s="0">
-        <v>-40161.07373046875</v>
+        <v>-3820.0561218261719</v>
       </c>
       <c r="C19" s="0">
-        <v>-40710.552093505859</v>
+        <v>-3322.888916015625</v>
       </c>
       <c r="D19" s="0">
-        <v>-37434.630737304688</v>
+        <v>-2351.6778259277344</v>
       </c>
       <c r="E19" s="0">
-        <v>-49382.434692382813</v>
+        <v>-8068.1610412597656</v>
       </c>
       <c r="F19" s="0">
-        <v>-62998.238372802734</v>
+        <v>-15259.358123779297</v>
       </c>
       <c r="G19" s="0">
-        <v>-62174.965293884277</v>
+        <v>-31389.453453063965</v>
       </c>
       <c r="H19" s="0">
-        <v>-58393.468208312988</v>
+        <v>-24877.609756469727</v>
       </c>
       <c r="I19" s="0">
-        <v>-54777.696144104004</v>
+        <v>-18858.205505371094</v>
       </c>
     </row>
     <row r="20">
@@ -902,28 +902,28 @@
         <v>19</v>
       </c>
       <c r="B20" s="0">
-        <v>-3320.0592422485352</v>
+        <v>1026.1051483154297</v>
       </c>
       <c r="C20" s="0">
-        <v>-3116.3677062988281</v>
+        <v>1515.5273513793945</v>
       </c>
       <c r="D20" s="0">
-        <v>-3323.7570304870605</v>
+        <v>1563.1033515930176</v>
       </c>
       <c r="E20" s="0">
-        <v>-4379.7850723266602</v>
+        <v>1057.626091003418</v>
       </c>
       <c r="F20" s="0">
-        <v>-5195.8923950195312</v>
+        <v>492.75648498535156</v>
       </c>
       <c r="G20" s="0">
-        <v>-13090.080960154533</v>
+        <v>-6512.5988540649414</v>
       </c>
       <c r="H20" s="0">
-        <v>-13775.762996673584</v>
+        <v>-7959.7619180679321</v>
       </c>
       <c r="I20" s="0">
-        <v>-14876.393232345581</v>
+        <v>-10772.969390869141</v>
       </c>
     </row>
     <row r="21">
@@ -931,28 +931,28 @@
         <v>20</v>
       </c>
       <c r="B21" s="0">
-        <v>-26520.754058837891</v>
+        <v>-25540.966674804688</v>
       </c>
       <c r="C21" s="0">
-        <v>-22067.936798095703</v>
+        <v>-21088.858703613281</v>
       </c>
       <c r="D21" s="0">
-        <v>-19726.573699951172</v>
+        <v>-18625.171173095703</v>
       </c>
       <c r="E21" s="0">
-        <v>-17928.22943687439</v>
+        <v>-17302.065313339233</v>
       </c>
       <c r="F21" s="0">
-        <v>-15357.895111083984</v>
+        <v>-14850.718780517578</v>
       </c>
       <c r="G21" s="0">
-        <v>-16158.260894775391</v>
+        <v>-14331.034408569336</v>
       </c>
       <c r="H21" s="0">
-        <v>-22924.297302246094</v>
+        <v>-20759.2568359375</v>
       </c>
       <c r="I21" s="0">
-        <v>-32147.319030761719</v>
+        <v>-29757.075897216797</v>
       </c>
     </row>
     <row r="22">
@@ -960,28 +960,28 @@
         <v>21</v>
       </c>
       <c r="B22" s="0">
-        <v>6384.9063568115234</v>
+        <v>13882.005233764648</v>
       </c>
       <c r="C22" s="0">
-        <v>2378.1885833740234</v>
+        <v>9642.7748718261719</v>
       </c>
       <c r="D22" s="0">
-        <v>143.09455108642578</v>
+        <v>7047.9986114501953</v>
       </c>
       <c r="E22" s="0">
-        <v>-4991.7893524169922</v>
+        <v>3712.26904296875</v>
       </c>
       <c r="F22" s="0">
-        <v>-309.27815246582031</v>
+        <v>15138.479614257813</v>
       </c>
       <c r="G22" s="0">
-        <v>-5113.9360466003418</v>
+        <v>15960.227832794189</v>
       </c>
       <c r="H22" s="0">
-        <v>-17014.24947977066</v>
+        <v>7019.5049591064453</v>
       </c>
       <c r="I22" s="0">
-        <v>-13547.44838142395</v>
+        <v>10281.635133743286</v>
       </c>
     </row>
     <row r="23">
@@ -989,28 +989,28 @@
         <v>22</v>
       </c>
       <c r="B23" s="0">
-        <v>-88294.524310112</v>
+        <v>-84628.282608032227</v>
       </c>
       <c r="C23" s="0">
-        <v>-96400.258969306946</v>
+        <v>-92589.953582763672</v>
       </c>
       <c r="D23" s="0">
-        <v>-94362.948956489563</v>
+        <v>-90758.899101257324</v>
       </c>
       <c r="E23" s="0">
-        <v>-99686.808015346527</v>
+        <v>-95561.779571533203</v>
       </c>
       <c r="F23" s="0">
-        <v>-115058.21760559082</v>
+        <v>-110369.8620300293</v>
       </c>
       <c r="G23" s="0">
-        <v>-110709.59186553955</v>
+        <v>-107885.99664306641</v>
       </c>
       <c r="H23" s="0">
-        <v>-130709.33515167236</v>
+        <v>-127965.4654083252</v>
       </c>
       <c r="I23" s="0">
-        <v>-131051.13106536865</v>
+        <v>-132136.30387878418</v>
       </c>
     </row>
     <row r="24">
@@ -1018,28 +1018,28 @@
         <v>23</v>
       </c>
       <c r="B24" s="0">
-        <v>-607.944091796875</v>
+        <v>-5388.6255798339844</v>
       </c>
       <c r="C24" s="0">
-        <v>-430.08849334716797</v>
+        <v>-5431.1697845458984</v>
       </c>
       <c r="D24" s="0">
-        <v>-4907.6849975585937</v>
+        <v>-9592.0480499267578</v>
       </c>
       <c r="E24" s="0">
-        <v>-2069.5505065917969</v>
+        <v>-7956.9535980224609</v>
       </c>
       <c r="F24" s="0">
-        <v>1379.7548217773437</v>
+        <v>-5539.9528865814209</v>
       </c>
       <c r="G24" s="0">
-        <v>4758.6175575256348</v>
+        <v>1849.4055671691895</v>
       </c>
       <c r="H24" s="0">
-        <v>-2912.7736396789551</v>
+        <v>-6035.7477922439575</v>
       </c>
       <c r="I24" s="0">
-        <v>3593.7501773834229</v>
+        <v>-33.578590393066406</v>
       </c>
     </row>
     <row r="25">
@@ -1047,28 +1047,28 @@
         <v>24</v>
       </c>
       <c r="B25" s="0">
-        <v>-13838.847068786621</v>
+        <v>-14213.023979187012</v>
       </c>
       <c r="C25" s="0">
-        <v>-15550.053894042969</v>
+        <v>-16043.482902526855</v>
       </c>
       <c r="D25" s="0">
-        <v>-17363.722640991211</v>
+        <v>-17544.197105407715</v>
       </c>
       <c r="E25" s="0">
-        <v>-19894.04296875</v>
+        <v>-20405.124404907227</v>
       </c>
       <c r="F25" s="0">
-        <v>-23555.301162719727</v>
+        <v>-24552.786987304688</v>
       </c>
       <c r="G25" s="0">
-        <v>-30350.118827819824</v>
+        <v>-33566.800685882568</v>
       </c>
       <c r="H25" s="0">
-        <v>-32307.932941436768</v>
+        <v>-36163.126609802246</v>
       </c>
       <c r="I25" s="0">
-        <v>-33504.014381408691</v>
+        <v>-37846.779006958008</v>
       </c>
     </row>
     <row r="26">
@@ -1076,28 +1076,28 @@
         <v>25</v>
       </c>
       <c r="B26" s="0">
-        <v>-3075.0254173278809</v>
+        <v>-7576.570761680603</v>
       </c>
       <c r="C26" s="0">
-        <v>-4958.8907470703125</v>
+        <v>-9643.5309181213379</v>
       </c>
       <c r="D26" s="0">
-        <v>-8272.8542327880859</v>
+        <v>-12646.002395629883</v>
       </c>
       <c r="E26" s="0">
-        <v>-9083.5026321411133</v>
+        <v>-14243.217811584473</v>
       </c>
       <c r="F26" s="0">
-        <v>-9654.7835845947266</v>
+        <v>-15538.805320739746</v>
       </c>
       <c r="G26" s="0">
-        <v>-5696.9903411865234</v>
+        <v>-11667.886764526367</v>
       </c>
       <c r="H26" s="0">
-        <v>-5296.3836517333984</v>
+        <v>-11835.965270996094</v>
       </c>
       <c r="I26" s="0">
-        <v>-6946.5235900878906</v>
+        <v>-14177.316665649414</v>
       </c>
     </row>
     <row r="27">
@@ -1105,28 +1105,28 @@
         <v>26</v>
       </c>
       <c r="B27" s="0">
-        <v>-7746.4558279514313</v>
+        <v>-9358.7011857032776</v>
       </c>
       <c r="C27" s="0">
-        <v>-8234.2300091981888</v>
+        <v>-9835.0782210826874</v>
       </c>
       <c r="D27" s="0">
-        <v>-7890.5097024440765</v>
+        <v>-9224.5674560815096</v>
       </c>
       <c r="E27" s="0">
-        <v>-8550.3059086799622</v>
+        <v>-10496.522656083107</v>
       </c>
       <c r="F27" s="0">
-        <v>-8863.8852751255035</v>
+        <v>-11121.087598562241</v>
       </c>
       <c r="G27" s="0">
-        <v>-10539.768211364746</v>
+        <v>-13188.714195251465</v>
       </c>
       <c r="H27" s="0">
-        <v>-10044.129852294922</v>
+        <v>-13093.460777282715</v>
       </c>
       <c r="I27" s="0">
-        <v>-9689.0746650695801</v>
+        <v>-13701.195899963379</v>
       </c>
     </row>
     <row r="28">
@@ -1134,28 +1134,28 @@
         <v>27</v>
       </c>
       <c r="B28" s="0">
-        <v>7310.7503280639648</v>
+        <v>7210.4086685180664</v>
       </c>
       <c r="C28" s="0">
-        <v>7582.8299789428711</v>
+        <v>7531.6462097167969</v>
       </c>
       <c r="D28" s="0">
-        <v>7950.4878082275391</v>
+        <v>7892.4452819824219</v>
       </c>
       <c r="E28" s="0">
-        <v>9198.9799728393555</v>
+        <v>9155.2227725982666</v>
       </c>
       <c r="F28" s="0">
-        <v>9150.7618064880371</v>
+        <v>9225.6617469787598</v>
       </c>
       <c r="G28" s="0">
-        <v>13464.8458776474</v>
+        <v>6538.0437707901001</v>
       </c>
       <c r="H28" s="0">
-        <v>15030.101021766663</v>
+        <v>7727.2571306228638</v>
       </c>
       <c r="I28" s="0">
-        <v>19336.462066650391</v>
+        <v>10851.983947753906</v>
       </c>
     </row>
     <row r="29">
@@ -1163,28 +1163,28 @@
         <v>28</v>
       </c>
       <c r="B29" s="0">
-        <v>21397.447601318359</v>
+        <v>16615.08182144165</v>
       </c>
       <c r="C29" s="0">
-        <v>21813.0973777771</v>
+        <v>16882.086235046387</v>
       </c>
       <c r="D29" s="0">
-        <v>20359.290782928467</v>
+        <v>16065.764232635498</v>
       </c>
       <c r="E29" s="0">
-        <v>22599.163974761963</v>
+        <v>22479.844435691833</v>
       </c>
       <c r="F29" s="0">
-        <v>30620.044677734375</v>
+        <v>24270.523231506348</v>
       </c>
       <c r="G29" s="0">
-        <v>32400.333759307861</v>
+        <v>28915.020969390869</v>
       </c>
       <c r="H29" s="0">
-        <v>32798.454360961914</v>
+        <v>30593.833648681641</v>
       </c>
       <c r="I29" s="0">
-        <v>25493.663795471191</v>
+        <v>23478.403442382813</v>
       </c>
     </row>
     <row r="30">
@@ -1192,28 +1192,28 @@
         <v>29</v>
       </c>
       <c r="B30" s="0">
-        <v>-1597.6752636730671</v>
+        <v>-4827.1925251483917</v>
       </c>
       <c r="C30" s="0">
-        <v>-1410.7549866437912</v>
+        <v>-3854.7433519363403</v>
       </c>
       <c r="D30" s="0">
-        <v>-2184.0766834020615</v>
+        <v>643.30171430110931</v>
       </c>
       <c r="E30" s="0">
-        <v>-3642.4679315090179</v>
+        <v>-1164.2437233924866</v>
       </c>
       <c r="F30" s="0">
-        <v>-5660.475043296814</v>
+        <v>-18255.021490097046</v>
       </c>
       <c r="G30" s="0">
-        <v>-16575.725355148315</v>
+        <v>-29981.084300994873</v>
       </c>
       <c r="H30" s="0">
-        <v>-18818.238725662231</v>
+        <v>-35528.280490875244</v>
       </c>
       <c r="I30" s="0">
-        <v>-21936.883750915527</v>
+        <v>-38160.806457519531</v>
       </c>
     </row>
     <row r="31">
@@ -1221,28 +1221,28 @@
         <v>30</v>
       </c>
       <c r="B31" s="0">
-        <v>-47223.006317138672</v>
+        <v>-42763.714630126953</v>
       </c>
       <c r="C31" s="0">
-        <v>-51159.641754150391</v>
+        <v>-46353.41828918457</v>
       </c>
       <c r="D31" s="0">
-        <v>-50533.18798828125</v>
+        <v>-46360.917541503906</v>
       </c>
       <c r="E31" s="0">
-        <v>-63812.480651855469</v>
+        <v>-58467.210174560547</v>
       </c>
       <c r="F31" s="0">
-        <v>-80923.270050048828</v>
+        <v>-73653.572692871094</v>
       </c>
       <c r="G31" s="0">
-        <v>-82152.002136230469</v>
+        <v>-73660.013634204865</v>
       </c>
       <c r="H31" s="0">
-        <v>-86275.569213867188</v>
+        <v>-76762.860690116882</v>
       </c>
       <c r="I31" s="0">
-        <v>-92747.563400268555</v>
+        <v>-81907.739540100098</v>
       </c>
     </row>
     <row r="32">
@@ -1250,28 +1250,28 @@
         <v>31</v>
       </c>
       <c r="B32" s="0">
-        <v>-11622.528404712677</v>
+        <v>-12671.071590125561</v>
       </c>
       <c r="C32" s="0">
-        <v>-11421.182528972626</v>
+        <v>-12640.868709683418</v>
       </c>
       <c r="D32" s="0">
-        <v>-10225.505586147308</v>
+        <v>-11169.109682679176</v>
       </c>
       <c r="E32" s="0">
-        <v>-10152.08416557312</v>
+        <v>-10499.485339403152</v>
       </c>
       <c r="F32" s="0">
-        <v>-12305.120801210403</v>
+        <v>-13806.298299968243</v>
       </c>
       <c r="G32" s="0">
-        <v>-16304.043029785156</v>
+        <v>-17064.5263671875</v>
       </c>
       <c r="H32" s="0">
-        <v>-15250.86311340332</v>
+        <v>-17165.964767456055</v>
       </c>
       <c r="I32" s="0">
-        <v>-14086.498641967773</v>
+        <v>-15433.335388183594</v>
       </c>
     </row>
     <row r="33">
@@ -1279,28 +1279,28 @@
         <v>32</v>
       </c>
       <c r="B33" s="0">
-        <v>95433.579650878906</v>
+        <v>100532.49383544922</v>
       </c>
       <c r="C33" s="0">
-        <v>128777.20858764648</v>
+        <v>133753.26760864258</v>
       </c>
       <c r="D33" s="0">
-        <v>106118.15008544922</v>
+        <v>110737.33520507813</v>
       </c>
       <c r="E33" s="0">
-        <v>84473.548034667969</v>
+        <v>91392.525329589844</v>
       </c>
       <c r="F33" s="0">
-        <v>76206.04345703125</v>
+        <v>84864.202301025391</v>
       </c>
       <c r="G33" s="0">
-        <v>100175.51428222656</v>
+        <v>105315.27185058594</v>
       </c>
       <c r="H33" s="0">
-        <v>112079.44519042969</v>
+        <v>116641.02783203125</v>
       </c>
       <c r="I33" s="0">
-        <v>114961.92028808594</v>
+        <v>119584.01184082031</v>
       </c>
     </row>
     <row r="34">
@@ -1308,28 +1308,28 @@
         <v>33</v>
       </c>
       <c r="B34" s="0">
-        <v>4697.7923202514648</v>
+        <v>14182.692222595215</v>
       </c>
       <c r="C34" s="0">
-        <v>8045.8919525146484</v>
+        <v>17617.256546020508</v>
       </c>
       <c r="D34" s="0">
-        <v>12821.892904281616</v>
+        <v>23081.378540039063</v>
       </c>
       <c r="E34" s="0">
-        <v>11685.440348982811</v>
+        <v>21118.606475830078</v>
       </c>
       <c r="F34" s="0">
-        <v>12113.198396682739</v>
+        <v>20762.623523712158</v>
       </c>
       <c r="G34" s="0">
-        <v>8579.0830688476562</v>
+        <v>16892.024627685547</v>
       </c>
       <c r="H34" s="0">
-        <v>6389.5555725097656</v>
+        <v>17173.852157592773</v>
       </c>
       <c r="I34" s="0">
-        <v>-4116.2237396240234</v>
+        <v>6836.4491119384766</v>
       </c>
     </row>
     <row r="35">
@@ -1337,28 +1337,28 @@
         <v>34</v>
       </c>
       <c r="B35" s="0">
-        <v>1194.7631297111511</v>
+        <v>-1948.8611037731171</v>
       </c>
       <c r="C35" s="0">
-        <v>792.82576560974121</v>
+        <v>-2441.3446545600891</v>
       </c>
       <c r="D35" s="0">
-        <v>414.13041234016418</v>
+        <v>-2648.0301418304443</v>
       </c>
       <c r="E35" s="0">
-        <v>1164.1317210197449</v>
+        <v>-2459.462119102478</v>
       </c>
       <c r="F35" s="0">
-        <v>1602.4491968154907</v>
+        <v>-2577.0674374103546</v>
       </c>
       <c r="G35" s="0">
-        <v>-4748.9636631011963</v>
+        <v>-5395.562328338623</v>
       </c>
       <c r="H35" s="0">
-        <v>-4462.7816681861877</v>
+        <v>-5125.9856376647949</v>
       </c>
       <c r="I35" s="0">
-        <v>-3327.1012425422668</v>
+        <v>-4094.453483581543</v>
       </c>
     </row>
     <row r="36">
@@ -1366,28 +1366,28 @@
         <v>35</v>
       </c>
       <c r="B36" s="0">
-        <v>1785.0787811279297</v>
+        <v>2553.2492065429687</v>
       </c>
       <c r="C36" s="0">
-        <v>-5564.1850128173828</v>
+        <v>-4500.7132949829102</v>
       </c>
       <c r="D36" s="0">
-        <v>-553.67081451416016</v>
+        <v>421.17066955566406</v>
       </c>
       <c r="E36" s="0">
-        <v>-1331.551887512207</v>
+        <v>-60.441482543945313</v>
       </c>
       <c r="F36" s="0">
-        <v>-10191.112833023071</v>
+        <v>-8866.3256320953369</v>
       </c>
       <c r="G36" s="0">
-        <v>-23441.740325927734</v>
+        <v>-23351.905517578125</v>
       </c>
       <c r="H36" s="0">
-        <v>-35434.404388427734</v>
+        <v>-35662.624145507813</v>
       </c>
       <c r="I36" s="0">
-        <v>-36876.854797363281</v>
+        <v>-37511.05712890625</v>
       </c>
     </row>
     <row r="37">
@@ -1395,28 +1395,28 @@
         <v>36</v>
       </c>
       <c r="B37" s="0">
-        <v>-11020.266540527344</v>
+        <v>-9825.1687622070312</v>
       </c>
       <c r="C37" s="0">
-        <v>-9913.9115600585937</v>
+        <v>-8688.5989685058594</v>
       </c>
       <c r="D37" s="0">
-        <v>-9416.9039154052734</v>
+        <v>-8278.0393981933594</v>
       </c>
       <c r="E37" s="0">
-        <v>-12337.682632446289</v>
+        <v>-10959.444702148438</v>
       </c>
       <c r="F37" s="0">
-        <v>-13254.799591064453</v>
+        <v>-11571.940139770508</v>
       </c>
       <c r="G37" s="0">
-        <v>-23040.220231056213</v>
+        <v>-23488.608140945435</v>
       </c>
       <c r="H37" s="0">
-        <v>-22887.29200553894</v>
+        <v>-23408.807020187378</v>
       </c>
       <c r="I37" s="0">
-        <v>-24565.786434173584</v>
+        <v>-25174.147693634033</v>
       </c>
     </row>
     <row r="38">
@@ -1424,28 +1424,28 @@
         <v>37</v>
       </c>
       <c r="B38" s="0">
-        <v>-6687.2862434387207</v>
+        <v>-7017.3737678527832</v>
       </c>
       <c r="C38" s="0">
-        <v>-10083.336769104004</v>
+        <v>-10444.478565216064</v>
       </c>
       <c r="D38" s="0">
-        <v>-14404.796127319336</v>
+        <v>-14791.761688232422</v>
       </c>
       <c r="E38" s="0">
-        <v>-14883.502985358238</v>
+        <v>-15551.943724930286</v>
       </c>
       <c r="F38" s="0">
-        <v>-17276.737436771393</v>
+        <v>-17654.513919353485</v>
       </c>
       <c r="G38" s="0">
-        <v>-16688.550018310547</v>
+        <v>-18593.452819824219</v>
       </c>
       <c r="H38" s="0">
-        <v>-12516.460235595703</v>
+        <v>-14971.055953979492</v>
       </c>
       <c r="I38" s="0">
-        <v>-9306.0932312011719</v>
+        <v>-12055.127029418945</v>
       </c>
     </row>
     <row r="39">
@@ -1453,28 +1453,28 @@
         <v>38</v>
       </c>
       <c r="B39" s="0">
-        <v>-85268.958892822266</v>
+        <v>-78905.161560058594</v>
       </c>
       <c r="C39" s="0">
-        <v>-87054.032424926758</v>
+        <v>-80803.671691894531</v>
       </c>
       <c r="D39" s="0">
-        <v>-91350.465911865234</v>
+        <v>-85409.978088378906</v>
       </c>
       <c r="E39" s="0">
-        <v>-99793.473968505859</v>
+        <v>-92638.724853515625</v>
       </c>
       <c r="F39" s="0">
-        <v>-104111.59020996094</v>
+        <v>-96409.748107910156</v>
       </c>
       <c r="G39" s="0">
-        <v>-115036.60669708252</v>
+        <v>-108831.33557891846</v>
       </c>
       <c r="H39" s="0">
-        <v>-131773.95492553711</v>
+        <v>-124603.0443572998</v>
       </c>
       <c r="I39" s="0">
-        <v>-113461.31205749512</v>
+        <v>-108294.22067260742</v>
       </c>
     </row>
     <row r="40">
@@ -1482,28 +1482,28 @@
         <v>39</v>
       </c>
       <c r="B40" s="0">
-        <v>-3996.8241529464722</v>
+        <v>-3513.5922060012817</v>
       </c>
       <c r="C40" s="0">
-        <v>-4234.6293640136719</v>
+        <v>-3714.0717849731445</v>
       </c>
       <c r="D40" s="0">
-        <v>-3949.6087350845337</v>
+        <v>-3603.5685787200928</v>
       </c>
       <c r="E40" s="0">
-        <v>-3839.9326477050781</v>
+        <v>-2972.0908813476562</v>
       </c>
       <c r="F40" s="0">
-        <v>-4054.977294921875</v>
+        <v>-2917.1720962524414</v>
       </c>
       <c r="G40" s="0">
-        <v>-8451.5553512573242</v>
+        <v>-7383.3493041992187</v>
       </c>
       <c r="H40" s="0">
-        <v>-9313.5146484375</v>
+        <v>-7865.2681846618652</v>
       </c>
       <c r="I40" s="0">
-        <v>-11182.362968444824</v>
+        <v>-18340.33540725708</v>
       </c>
     </row>
     <row r="41">
@@ -1511,28 +1511,28 @@
         <v>40</v>
       </c>
       <c r="B41" s="0">
-        <v>-16903.978488922119</v>
+        <v>-14735.104831218719</v>
       </c>
       <c r="C41" s="0">
-        <v>-19946.399658203125</v>
+        <v>-17728.150508880615</v>
       </c>
       <c r="D41" s="0">
-        <v>-22528.675659179688</v>
+        <v>-20434.347719192505</v>
       </c>
       <c r="E41" s="0">
-        <v>-22542.815002441406</v>
+        <v>-19987.301723480225</v>
       </c>
       <c r="F41" s="0">
-        <v>-25005.14159488678</v>
+        <v>-21826.478538513184</v>
       </c>
       <c r="G41" s="0">
-        <v>-29113.909484863281</v>
+        <v>-27347.503387451172</v>
       </c>
       <c r="H41" s="0">
-        <v>-33979.311798095703</v>
+        <v>-32099.752014160156</v>
       </c>
       <c r="I41" s="0">
-        <v>-31821.500549316406</v>
+        <v>-29963.461837768555</v>
       </c>
     </row>
     <row r="42">
@@ -1540,28 +1540,28 @@
         <v>41</v>
       </c>
       <c r="B42" s="0">
-        <v>2993.0268079042435</v>
+        <v>-3003.1744194030762</v>
       </c>
       <c r="C42" s="0">
-        <v>4208.0117648243904</v>
+        <v>-1951.9556931257248</v>
       </c>
       <c r="D42" s="0">
-        <v>5794.9424302577972</v>
+        <v>637.49455440044403</v>
       </c>
       <c r="E42" s="0">
-        <v>6900.6470420062542</v>
+        <v>1855.2409725189209</v>
       </c>
       <c r="F42" s="0">
-        <v>7157.6945124268532</v>
+        <v>-2450.6491484642029</v>
       </c>
       <c r="G42" s="0">
-        <v>3254.5118970870972</v>
+        <v>-2321.4526195526123</v>
       </c>
       <c r="H42" s="0">
-        <v>3736.1684756278992</v>
+        <v>-2632.6102848052979</v>
       </c>
       <c r="I42" s="0">
-        <v>4577.0541734695435</v>
+        <v>1008.5012311935425</v>
       </c>
     </row>
     <row r="43">
@@ -1569,28 +1569,28 @@
         <v>42</v>
       </c>
       <c r="B43" s="0">
-        <v>17854.938385009766</v>
+        <v>18017.830902099609</v>
       </c>
       <c r="C43" s="0">
-        <v>16237.278198242188</v>
+        <v>16330.159515380859</v>
       </c>
       <c r="D43" s="0">
-        <v>15237.470916748047</v>
+        <v>15283.386169433594</v>
       </c>
       <c r="E43" s="0">
-        <v>16459.289520263672</v>
+        <v>17161.575988769531</v>
       </c>
       <c r="F43" s="0">
-        <v>16965.308898925781</v>
+        <v>18535.552062988281</v>
       </c>
       <c r="G43" s="0">
-        <v>97.680923461914063</v>
+        <v>2562.8612060546875</v>
       </c>
       <c r="H43" s="0">
-        <v>-1960.8292846679687</v>
+        <v>339.66347503662109</v>
       </c>
       <c r="I43" s="0">
-        <v>2230.13720703125</v>
+        <v>3069.7855682373047</v>
       </c>
     </row>
     <row r="44">
@@ -1598,28 +1598,28 @@
         <v>43</v>
       </c>
       <c r="B44" s="0">
-        <v>-86577.466918945313</v>
+        <v>-77666.251953125</v>
       </c>
       <c r="C44" s="0">
-        <v>-97394.414123535156</v>
+        <v>-87960.006408691406</v>
       </c>
       <c r="D44" s="0">
-        <v>-110243.86184692383</v>
+        <v>-101116.6047668457</v>
       </c>
       <c r="E44" s="0">
-        <v>-131219.22280883789</v>
+        <v>-121630.77917480469</v>
       </c>
       <c r="F44" s="0">
-        <v>-153983.12916564941</v>
+        <v>-145056.18293762207</v>
       </c>
       <c r="G44" s="0">
-        <v>-153035.69606018066</v>
+        <v>-133660.08907318115</v>
       </c>
       <c r="H44" s="0">
-        <v>-138399.78564453125</v>
+        <v>-116491.34155273437</v>
       </c>
       <c r="I44" s="0">
-        <v>-99204.002685546875</v>
+        <v>-77039.11669921875</v>
       </c>
     </row>
     <row r="45">
@@ -1627,28 +1627,28 @@
         <v>44</v>
       </c>
       <c r="B45" s="0">
-        <v>8148.8801193237305</v>
+        <v>8680.9947814941406</v>
       </c>
       <c r="C45" s="0">
-        <v>8425.5569152832031</v>
+        <v>8848.6850509643555</v>
       </c>
       <c r="D45" s="0">
-        <v>7764.794246673584</v>
+        <v>8411.8773918151855</v>
       </c>
       <c r="E45" s="0">
-        <v>6847.1047134399414</v>
+        <v>6983.8034210205078</v>
       </c>
       <c r="F45" s="0">
-        <v>8086.1578407287598</v>
+        <v>8083.9723701477051</v>
       </c>
       <c r="G45" s="0">
-        <v>3980.8870105743408</v>
+        <v>4637.2296943664551</v>
       </c>
       <c r="H45" s="0">
-        <v>8785.3384094238281</v>
+        <v>8821.1183776855469</v>
       </c>
       <c r="I45" s="0">
-        <v>13528.525714874268</v>
+        <v>12192.425643920898</v>
       </c>
     </row>
     <row r="46">
@@ -1656,28 +1656,28 @@
         <v>45</v>
       </c>
       <c r="B46" s="0">
-        <v>-5285.6023409366608</v>
+        <v>-48708.96503508091</v>
       </c>
       <c r="C46" s="0">
-        <v>-5529.7337423563004</v>
+        <v>-49145.483642101288</v>
       </c>
       <c r="D46" s="0">
-        <v>-5150.5264620780945</v>
+        <v>-60869.692857265472</v>
       </c>
       <c r="E46" s="0">
-        <v>-5548.5326099395752</v>
+        <v>-65748.406996250153</v>
       </c>
       <c r="F46" s="0">
-        <v>-4938.1969928741455</v>
+        <v>-49816.011447906494</v>
       </c>
       <c r="G46" s="0">
-        <v>-6602.9085693359375</v>
+        <v>-61026.280334472656</v>
       </c>
       <c r="H46" s="0">
-        <v>-8753.3727035522461</v>
+        <v>-61742.086456298828</v>
       </c>
       <c r="I46" s="0">
-        <v>-8798.9333305358887</v>
+        <v>-57027.74235534668</v>
       </c>
     </row>
     <row r="47">
@@ -1685,28 +1685,28 @@
         <v>46</v>
       </c>
       <c r="B47" s="0">
-        <v>2151.3548240661621</v>
+        <v>4182.5747604370117</v>
       </c>
       <c r="C47" s="0">
-        <v>6730.5080413818359</v>
+        <v>8440.7006988525391</v>
       </c>
       <c r="D47" s="0">
-        <v>6876.500415802002</v>
+        <v>8564.8912048339844</v>
       </c>
       <c r="E47" s="0">
-        <v>8629.4409618377686</v>
+        <v>10663.400672912598</v>
       </c>
       <c r="F47" s="0">
-        <v>6526.2108306884766</v>
+        <v>22570.256034851074</v>
       </c>
       <c r="G47" s="0">
-        <v>-8727.8790893554687</v>
+        <v>7580.0736999511719</v>
       </c>
       <c r="H47" s="0">
-        <v>-11361.937438964844</v>
+        <v>-4646.6982421875</v>
       </c>
       <c r="I47" s="0">
-        <v>-17448.712280273438</v>
+        <v>-5341.4580688476562</v>
       </c>
     </row>
     <row r="48">
@@ -1714,28 +1714,28 @@
         <v>47</v>
       </c>
       <c r="B48" s="0">
-        <v>2747.1143798828125</v>
+        <v>9173.5325927734375</v>
       </c>
       <c r="C48" s="0">
-        <v>1169.7434997558594</v>
+        <v>7770.9726867675781</v>
       </c>
       <c r="D48" s="0">
-        <v>1027.6587524414062</v>
+        <v>7516.1102600097656</v>
       </c>
       <c r="E48" s="0">
-        <v>744.23162841796875</v>
+        <v>8552.9668273925781</v>
       </c>
       <c r="F48" s="0">
-        <v>-17377.057250976563</v>
+        <v>-7103.5252990722656</v>
       </c>
       <c r="G48" s="0">
-        <v>-16749.668452262878</v>
+        <v>-7613.6840772628784</v>
       </c>
       <c r="H48" s="0">
-        <v>-9175.384521484375</v>
+        <v>445.753662109375</v>
       </c>
       <c r="I48" s="0">
-        <v>14600.647277832031</v>
+        <v>26090.999206542969</v>
       </c>
     </row>
     <row r="49">
@@ -1743,28 +1743,28 @@
         <v>48</v>
       </c>
       <c r="B49" s="0">
-        <v>-8683.0030212402344</v>
+        <v>-18126.042163848877</v>
       </c>
       <c r="C49" s="0">
-        <v>-9337.3157138824463</v>
+        <v>-18721.30838394165</v>
       </c>
       <c r="D49" s="0">
-        <v>-9997.4310207366943</v>
+        <v>-18540.458452224731</v>
       </c>
       <c r="E49" s="0">
-        <v>-11235.33900642395</v>
+        <v>-21752.779907226563</v>
       </c>
       <c r="F49" s="0">
-        <v>-11994.600337982178</v>
+        <v>-26747.666496276855</v>
       </c>
       <c r="G49" s="0">
-        <v>-17229.33610534668</v>
+        <v>-33630.20189666748</v>
       </c>
       <c r="H49" s="0">
-        <v>-17611.468360900879</v>
+        <v>-30573.62186050415</v>
       </c>
       <c r="I49" s="0">
-        <v>-17273.583953857422</v>
+        <v>-27422.723739624023</v>
       </c>
     </row>
     <row r="50">
@@ -1772,28 +1772,28 @@
         <v>49</v>
       </c>
       <c r="B50" s="0">
-        <v>-10272.281513214111</v>
+        <v>-8813.0845794677734</v>
       </c>
       <c r="C50" s="0">
-        <v>-10895.909069061279</v>
+        <v>-9424.0874366760254</v>
       </c>
       <c r="D50" s="0">
-        <v>-11986.671447753906</v>
+        <v>-10587.596378326416</v>
       </c>
       <c r="E50" s="0">
-        <v>-14905.985359191895</v>
+        <v>-13118.48193359375</v>
       </c>
       <c r="F50" s="0">
-        <v>-16644.550521850586</v>
+        <v>-14807.881805419922</v>
       </c>
       <c r="G50" s="0">
-        <v>-20617.465099334717</v>
+        <v>-21161.876045227051</v>
       </c>
       <c r="H50" s="0">
-        <v>-25932.227806091309</v>
+        <v>-26585.205177307129</v>
       </c>
       <c r="I50" s="0">
-        <v>-25237.726226806641</v>
+        <v>-25693.603607177734</v>
       </c>
     </row>
     <row r="51">
@@ -1801,28 +1801,28 @@
         <v>50</v>
       </c>
       <c r="B51" s="0">
-        <v>-3211.3713140487671</v>
+        <v>-6731.4952955245972</v>
       </c>
       <c r="C51" s="0">
-        <v>-3383.9297323226929</v>
+        <v>-6966.1852216720581</v>
       </c>
       <c r="D51" s="0">
-        <v>-2901.3328428268433</v>
+        <v>-7195.1884489059448</v>
       </c>
       <c r="E51" s="0">
-        <v>-3654.9297752380371</v>
+        <v>-9701.3515796661377</v>
       </c>
       <c r="F51" s="0">
-        <v>-4446.9866714477539</v>
+        <v>-9652.6853466033936</v>
       </c>
       <c r="G51" s="0">
-        <v>-5761.3656883239746</v>
+        <v>-9743.1819581985474</v>
       </c>
       <c r="H51" s="0">
-        <v>-5025.7318229675293</v>
+        <v>-7572.8228092193604</v>
       </c>
       <c r="I51" s="0">
-        <v>-4396.1925029754639</v>
+        <v>-6845.2044401168823</v>
       </c>
     </row>
     <row r="52">
@@ -1830,28 +1830,28 @@
         <v>51</v>
       </c>
       <c r="B52" s="0">
-        <v>6798.1544189453125</v>
+        <v>6606.9892578125</v>
       </c>
       <c r="C52" s="0">
-        <v>5343.5125503540039</v>
+        <v>5278.9022827148437</v>
       </c>
       <c r="D52" s="0">
-        <v>-3281.5405883789062</v>
+        <v>-3218.6171264648437</v>
       </c>
       <c r="E52" s="0">
-        <v>-7585.7089233398437</v>
+        <v>-7535.2294311523437</v>
       </c>
       <c r="F52" s="0">
-        <v>-8851.3941040039062</v>
+        <v>-8753.6112670898437</v>
       </c>
       <c r="G52" s="0">
-        <v>-2204.5242919921875</v>
+        <v>-2173.9556884765625</v>
       </c>
       <c r="H52" s="0">
-        <v>227.884765625</v>
+        <v>230.91064453125</v>
       </c>
       <c r="I52" s="0">
-        <v>-8075.9931640625</v>
+        <v>-8139.63525390625</v>
       </c>
     </row>
     <row r="53">
@@ -1859,28 +1859,28 @@
         <v>52</v>
       </c>
       <c r="B53" s="0">
-        <v>2381.7510986328125</v>
+        <v>2167.5977783203125</v>
       </c>
       <c r="C53" s="0">
-        <v>3279.8279161453247</v>
+        <v>3078.5483751296997</v>
       </c>
       <c r="D53" s="0">
-        <v>7795.5922644138336</v>
+        <v>7595.5737097263336</v>
       </c>
       <c r="E53" s="0">
-        <v>6528.3671188354492</v>
+        <v>6288.6543502807617</v>
       </c>
       <c r="F53" s="0">
-        <v>8650.9976482391357</v>
+        <v>8403.6961345672607</v>
       </c>
       <c r="G53" s="0">
-        <v>9949.8118362426758</v>
+        <v>9724.5043411254883</v>
       </c>
       <c r="H53" s="0">
-        <v>15230.469818115234</v>
+        <v>14968.844940185547</v>
       </c>
       <c r="I53" s="0">
-        <v>19419.496109008789</v>
+        <v>19068.479263305664</v>
       </c>
     </row>
     <row r="54">
@@ -1888,28 +1888,28 @@
         <v>53</v>
       </c>
       <c r="B54" s="0">
-        <v>14154.832260131836</v>
+        <v>14150.896224975586</v>
       </c>
       <c r="C54" s="0">
-        <v>15829.644256591797</v>
+        <v>15771.904754638672</v>
       </c>
       <c r="D54" s="0">
-        <v>20425.387494087219</v>
+        <v>20448.356122016907</v>
       </c>
       <c r="E54" s="0">
-        <v>25303.674812316895</v>
+        <v>25313.944831848145</v>
       </c>
       <c r="F54" s="0">
-        <v>28021.084884643555</v>
+        <v>28006.646408081055</v>
       </c>
       <c r="G54" s="0">
-        <v>25497.075378417969</v>
+        <v>25489.697448730469</v>
       </c>
       <c r="H54" s="0">
-        <v>28064.847076416016</v>
+        <v>28018.590240478516</v>
       </c>
       <c r="I54" s="0">
-        <v>32236.427642822266</v>
+        <v>32200.504058837891</v>
       </c>
     </row>
     <row r="55">
@@ -1917,28 +1917,28 @@
         <v>54</v>
       </c>
       <c r="B55" s="0">
-        <v>-661.85416412353516</v>
+        <v>-731.43885040283203</v>
       </c>
       <c r="C55" s="0">
-        <v>-1338.0202722549438</v>
+        <v>-1401.8055505752563</v>
       </c>
       <c r="D55" s="0">
-        <v>-1511.4333252906799</v>
+        <v>-1574.5061707496643</v>
       </c>
       <c r="E55" s="0">
-        <v>-2190.3480129241943</v>
+        <v>-2268.5954723358154</v>
       </c>
       <c r="F55" s="0">
-        <v>-2888.7333374023437</v>
+        <v>-2977.7669219970703</v>
       </c>
       <c r="G55" s="0">
-        <v>-3950.546085357666</v>
+        <v>-4027.0927581787109</v>
       </c>
       <c r="H55" s="0">
-        <v>-3132.9857635498047</v>
+        <v>-3209.0272750854492</v>
       </c>
       <c r="I55" s="0">
-        <v>-7867.6702194213867</v>
+        <v>-7984.2428207397461</v>
       </c>
     </row>
     <row r="56">
@@ -1946,28 +1946,28 @@
         <v>55</v>
       </c>
       <c r="B56" s="0">
-        <v>-5482.6755981445312</v>
+        <v>-5587.5285034179687</v>
       </c>
       <c r="C56" s="0">
-        <v>-1582.4599609375</v>
+        <v>-1447.4080810546875</v>
       </c>
       <c r="D56" s="0">
-        <v>12367.406188964844</v>
+        <v>12549.401306152344</v>
       </c>
       <c r="E56" s="0">
-        <v>20670.993587493896</v>
+        <v>21023.932682037354</v>
       </c>
       <c r="F56" s="0">
-        <v>31221.450238227844</v>
+        <v>32063.368026733398</v>
       </c>
       <c r="G56" s="0">
-        <v>38323.904373168945</v>
+        <v>39009.06965637207</v>
       </c>
       <c r="H56" s="0">
-        <v>39531.285186767578</v>
+        <v>40031.845855712891</v>
       </c>
       <c r="I56" s="0">
-        <v>30899.167625427246</v>
+        <v>31381.601684570313</v>
       </c>
     </row>
     <row r="57">
@@ -1975,28 +1975,28 @@
         <v>56</v>
       </c>
       <c r="B57" s="0">
-        <v>54775.923278808594</v>
+        <v>75973.614685058594</v>
       </c>
       <c r="C57" s="0">
-        <v>52950.3486328125</v>
+        <v>73304.29052734375</v>
       </c>
       <c r="D57" s="0">
-        <v>44144.767944335938</v>
+        <v>64133.250854492188</v>
       </c>
       <c r="E57" s="0">
-        <v>46315.170104980469</v>
+        <v>68892.614685058594</v>
       </c>
       <c r="F57" s="0">
-        <v>58179.58447265625</v>
+        <v>81110.61669921875</v>
       </c>
       <c r="G57" s="0">
-        <v>58805.782196044922</v>
+        <v>84222.164520263672</v>
       </c>
       <c r="H57" s="0">
-        <v>50188.626953125</v>
+        <v>78973.96337890625</v>
       </c>
       <c r="I57" s="0">
-        <v>46985.40478515625</v>
+        <v>78546.72509765625</v>
       </c>
     </row>
     <row r="58">
@@ -2004,28 +2004,28 @@
         <v>57</v>
       </c>
       <c r="B58" s="0">
-        <v>45177.370758056641</v>
+        <v>44329.797760009766</v>
       </c>
       <c r="C58" s="0">
-        <v>45847.081359863281</v>
+        <v>44996.867248535156</v>
       </c>
       <c r="D58" s="0">
-        <v>58811.393798828125</v>
+        <v>57913.740966796875</v>
       </c>
       <c r="E58" s="0">
-        <v>65431.626953125</v>
+        <v>65101.725830078125</v>
       </c>
       <c r="F58" s="0">
-        <v>87998.538146972656</v>
+        <v>88349.568420410156</v>
       </c>
       <c r="G58" s="0">
-        <v>170376.99523925781</v>
+        <v>170009.79211425781</v>
       </c>
       <c r="H58" s="0">
-        <v>265326.82255554199</v>
+        <v>264443.19755554199</v>
       </c>
       <c r="I58" s="0">
-        <v>377199.07907104492</v>
+        <v>375770.66696166992</v>
       </c>
     </row>
     <row r="59">
@@ -2033,28 +2033,28 @@
         <v>58</v>
       </c>
       <c r="B59" s="0">
-        <v>-2038.1047053337097</v>
+        <v>-2036.8886485099792</v>
       </c>
       <c r="C59" s="0">
-        <v>-2082.9458165168762</v>
+        <v>-2082.9974484443665</v>
       </c>
       <c r="D59" s="0">
-        <v>-2396.1793812513351</v>
+        <v>-2396.9597538709641</v>
       </c>
       <c r="E59" s="0">
-        <v>-2703.5645198822021</v>
+        <v>-2688.7443065643311</v>
       </c>
       <c r="F59" s="0">
-        <v>-2972.3768844604492</v>
+        <v>-2977.1576156616211</v>
       </c>
       <c r="G59" s="0">
-        <v>-3129.3685760498047</v>
+        <v>-3134.7769927978516</v>
       </c>
       <c r="H59" s="0">
-        <v>-3728.2191543579102</v>
+        <v>-3730.7346076965332</v>
       </c>
       <c r="I59" s="0">
-        <v>-4939.4412231445312</v>
+        <v>-4944.2386856079102</v>
       </c>
     </row>
     <row r="60">
@@ -2062,28 +2062,28 @@
         <v>59</v>
       </c>
       <c r="B60" s="0">
-        <v>-1742.0237350463867</v>
+        <v>-1885.4361343383789</v>
       </c>
       <c r="C60" s="0">
-        <v>-1570.6284637451172</v>
+        <v>-1721.9160614013672</v>
       </c>
       <c r="D60" s="0">
-        <v>-1167.1207885742187</v>
+        <v>-1326.1422424316406</v>
       </c>
       <c r="E60" s="0">
-        <v>-1517.5311279296875</v>
+        <v>-1702.0271606445312</v>
       </c>
       <c r="F60" s="0">
-        <v>846.22781372070312</v>
+        <v>642.45510864257813</v>
       </c>
       <c r="G60" s="0">
-        <v>3977.8755340576172</v>
+        <v>3801.3812408447266</v>
       </c>
       <c r="H60" s="0">
-        <v>4923.7522373199463</v>
+        <v>4706.7772617340088</v>
       </c>
       <c r="I60" s="0">
-        <v>9168.66455078125</v>
+        <v>8885.0066528320312</v>
       </c>
     </row>
     <row r="61">
@@ -2091,28 +2091,28 @@
         <v>60</v>
       </c>
       <c r="B61" s="0">
-        <v>68039.660400390625</v>
+        <v>67272.499267578125</v>
       </c>
       <c r="C61" s="0">
-        <v>93285.436889648438</v>
+        <v>92551.567260742188</v>
       </c>
       <c r="D61" s="0">
-        <v>144437.74645996094</v>
+        <v>143811.73278808594</v>
       </c>
       <c r="E61" s="0">
-        <v>166017.04968261719</v>
+        <v>165241.03845214844</v>
       </c>
       <c r="F61" s="0">
-        <v>213051.20740318298</v>
+        <v>212267.52869224548</v>
       </c>
       <c r="G61" s="0">
-        <v>224325.71459960938</v>
+        <v>223517.04516601563</v>
       </c>
       <c r="H61" s="0">
-        <v>240592.5654296875</v>
+        <v>239604.28759765625</v>
       </c>
       <c r="I61" s="0">
-        <v>322422.0433807373</v>
+        <v>320930.3314666748</v>
       </c>
     </row>
     <row r="62">
@@ -2120,28 +2120,28 @@
         <v>61</v>
       </c>
       <c r="B62" s="0">
-        <v>11364.716824531555</v>
+        <v>11109.355557441711</v>
       </c>
       <c r="C62" s="0">
-        <v>12126.929473876953</v>
+        <v>11875.606962203979</v>
       </c>
       <c r="D62" s="0">
-        <v>11920.183300018311</v>
+        <v>11697.132930755615</v>
       </c>
       <c r="E62" s="0">
-        <v>15192.028137207031</v>
+        <v>14938.008541107178</v>
       </c>
       <c r="F62" s="0">
-        <v>14438.119026184082</v>
+        <v>14191.415357589722</v>
       </c>
       <c r="G62" s="0">
-        <v>15027.602897644043</v>
+        <v>14807.256935119629</v>
       </c>
       <c r="H62" s="0">
-        <v>11123.814727783203</v>
+        <v>10911.216369628906</v>
       </c>
       <c r="I62" s="0">
-        <v>11101.242176055908</v>
+        <v>10758.945957183838</v>
       </c>
     </row>
     <row r="63">
@@ -2149,28 +2149,28 @@
         <v>62</v>
       </c>
       <c r="B63" s="0">
-        <v>-34031.767448425293</v>
+        <v>-33992.643394470215</v>
       </c>
       <c r="C63" s="0">
-        <v>-32308.736640930176</v>
+        <v>-32142.190803527832</v>
       </c>
       <c r="D63" s="0">
-        <v>-33193.200008392334</v>
+        <v>-32987.057064056396</v>
       </c>
       <c r="E63" s="0">
-        <v>-44037.650726318359</v>
+        <v>-43755.204254150391</v>
       </c>
       <c r="F63" s="0">
-        <v>-65792.061645507813</v>
+        <v>-65577.454345703125</v>
       </c>
       <c r="G63" s="0">
-        <v>-82445.28076171875</v>
+        <v>-82288.880615234375</v>
       </c>
       <c r="H63" s="0">
-        <v>-100401.07403564453</v>
+        <v>-100255.91705322266</v>
       </c>
       <c r="I63" s="0">
-        <v>-121488.39093017578</v>
+        <v>-121101.44830322266</v>
       </c>
     </row>
     <row r="64">
@@ -2178,28 +2178,28 @@
         <v>63</v>
       </c>
       <c r="B64" s="0">
-        <v>-621.38583374023437</v>
+        <v>-653.007399559021</v>
       </c>
       <c r="C64" s="0">
-        <v>-1459.8885188102722</v>
+        <v>-1495.7436027526855</v>
       </c>
       <c r="D64" s="0">
-        <v>-916.66977310180664</v>
+        <v>-957.58738708496094</v>
       </c>
       <c r="E64" s="0">
-        <v>-1725.5776062011719</v>
+        <v>-1776.6353073120117</v>
       </c>
       <c r="F64" s="0">
-        <v>-2344.152027130127</v>
+        <v>-2429.8435249328613</v>
       </c>
       <c r="G64" s="0">
-        <v>-1880.7276077270508</v>
+        <v>-1959.3654556274414</v>
       </c>
       <c r="H64" s="0">
-        <v>-2115.6341285705566</v>
+        <v>-2182.7989387512207</v>
       </c>
       <c r="I64" s="0">
-        <v>-2817.400803565979</v>
+        <v>-2916.8617486953735</v>
       </c>
     </row>
     <row r="65">
@@ -2207,28 +2207,28 @@
         <v>64</v>
       </c>
       <c r="B65" s="0">
-        <v>13079.556381225586</v>
+        <v>12861.505294799805</v>
       </c>
       <c r="C65" s="0">
-        <v>13627.783794641495</v>
+        <v>13376.880535364151</v>
       </c>
       <c r="D65" s="0">
-        <v>14502.030620574951</v>
+        <v>14226.039287567139</v>
       </c>
       <c r="E65" s="0">
-        <v>13748.487159729004</v>
+        <v>13432.346900939941</v>
       </c>
       <c r="F65" s="0">
-        <v>15408.267351150513</v>
+        <v>15104.09388923645</v>
       </c>
       <c r="G65" s="0">
-        <v>11722.897766113281</v>
+        <v>11418.203491210938</v>
       </c>
       <c r="H65" s="0">
-        <v>13859.371612548828</v>
+        <v>13551.673980712891</v>
       </c>
       <c r="I65" s="0">
-        <v>16974.862487792969</v>
+        <v>16513.059265136719</v>
       </c>
     </row>
     <row r="66">
@@ -2236,28 +2236,28 @@
         <v>65</v>
       </c>
       <c r="B66" s="0">
-        <v>20213.4375</v>
+        <v>19946.922546386719</v>
       </c>
       <c r="C66" s="0">
-        <v>20737.07177734375</v>
+        <v>20440.316619873047</v>
       </c>
       <c r="D66" s="0">
-        <v>25297.222381591797</v>
+        <v>25153.171112060547</v>
       </c>
       <c r="E66" s="0">
-        <v>22206.869781494141</v>
+        <v>21987.166168212891</v>
       </c>
       <c r="F66" s="0">
-        <v>13693.211303710938</v>
+        <v>13549.397827148438</v>
       </c>
       <c r="G66" s="0">
-        <v>-3639.4297561645508</v>
+        <v>-3731.2422561645508</v>
       </c>
       <c r="H66" s="0">
-        <v>-12691.825675964355</v>
+        <v>-12757.615226745605</v>
       </c>
       <c r="I66" s="0">
-        <v>-25087.414840698242</v>
+        <v>-25225.171188354492</v>
       </c>
     </row>
     <row r="67">
@@ -2265,28 +2265,28 @@
         <v>66</v>
       </c>
       <c r="B67" s="0">
-        <v>2787.3040084838867</v>
+        <v>1936.4985885620117</v>
       </c>
       <c r="C67" s="0">
-        <v>-3358.1769943237305</v>
+        <v>-4307.7463302612305</v>
       </c>
       <c r="D67" s="0">
-        <v>-9502.4814758300781</v>
+        <v>-10516.742706298828</v>
       </c>
       <c r="E67" s="0">
-        <v>-5736.9673767089844</v>
+        <v>-6962.8682556152344</v>
       </c>
       <c r="F67" s="0">
-        <v>-18357.793701171875</v>
+        <v>-19492.601806640625</v>
       </c>
       <c r="G67" s="0">
-        <v>-35219.509307861328</v>
+        <v>-36384.519409179688</v>
       </c>
       <c r="H67" s="0">
-        <v>-34746.634460449219</v>
+        <v>-36058.569091796875</v>
       </c>
       <c r="I67" s="0">
-        <v>-39809.393188476563</v>
+        <v>-41688.372680664063</v>
       </c>
     </row>
     <row r="68">
@@ -2294,28 +2294,28 @@
         <v>67</v>
       </c>
       <c r="B68" s="0">
-        <v>-22286.394088745117</v>
+        <v>-22502.157653808594</v>
       </c>
       <c r="C68" s="0">
-        <v>-22757.413021087646</v>
+        <v>-22938.224197387695</v>
       </c>
       <c r="D68" s="0">
-        <v>-26853.241149902344</v>
+        <v>-27058.880920410156</v>
       </c>
       <c r="E68" s="0">
-        <v>-30983.858154296875</v>
+        <v>-31254.158935546875</v>
       </c>
       <c r="F68" s="0">
-        <v>-31231.269958496094</v>
+        <v>-31520.938842773438</v>
       </c>
       <c r="G68" s="0">
-        <v>-30876.551879882813</v>
+        <v>-31114.836730957031</v>
       </c>
       <c r="H68" s="0">
-        <v>-36863.684997558594</v>
+        <v>-37142.8046875</v>
       </c>
       <c r="I68" s="0">
-        <v>-47748.664428710938</v>
+        <v>-48168.733032226563</v>
       </c>
     </row>
     <row r="69">
@@ -2323,28 +2323,28 @@
         <v>68</v>
       </c>
       <c r="B69" s="0">
-        <v>-2932.9896392822266</v>
+        <v>-3106.5684661865234</v>
       </c>
       <c r="C69" s="0">
-        <v>-2174.3219680786133</v>
+        <v>-2350.3413238525391</v>
       </c>
       <c r="D69" s="0">
-        <v>-1994.5252685546875</v>
+        <v>-2176.5518798828125</v>
       </c>
       <c r="E69" s="0">
-        <v>-3619.1003112792969</v>
+        <v>-3835.1083984375</v>
       </c>
       <c r="F69" s="0">
-        <v>-3506.4180068969727</v>
+        <v>-3731.0412368774414</v>
       </c>
       <c r="G69" s="0">
-        <v>-2330.0831298828125</v>
+        <v>-2526.0962524414062</v>
       </c>
       <c r="H69" s="0">
-        <v>-972.54544067382812</v>
+        <v>-1187.1187438964844</v>
       </c>
       <c r="I69" s="0">
-        <v>1648.7839126586914</v>
+        <v>1364.5552749633789</v>
       </c>
     </row>
     <row r="70">
@@ -2352,28 +2352,28 @@
         <v>69</v>
       </c>
       <c r="B70" s="0">
-        <v>18603.790649414063</v>
+        <v>18553.765563964844</v>
       </c>
       <c r="C70" s="0">
-        <v>16164.30419921875</v>
+        <v>16310.713012695313</v>
       </c>
       <c r="D70" s="0">
-        <v>15768.407836914062</v>
+        <v>15772.065063476563</v>
       </c>
       <c r="E70" s="0">
-        <v>20245.358825683594</v>
+        <v>20296.740173339844</v>
       </c>
       <c r="F70" s="0">
-        <v>15260.920104980469</v>
+        <v>15294.386901855469</v>
       </c>
       <c r="G70" s="0">
-        <v>15997.184753417969</v>
+        <v>15982.362609863281</v>
       </c>
       <c r="H70" s="0">
-        <v>24757.570587158203</v>
+        <v>24782.139190673828</v>
       </c>
       <c r="I70" s="0">
-        <v>23354.588150024414</v>
+        <v>23463.254653930664</v>
       </c>
     </row>
     <row r="71">
@@ -2381,28 +2381,28 @@
         <v>70</v>
       </c>
       <c r="B71" s="0">
-        <v>380.98666381835937</v>
+        <v>-2184.0218811035156</v>
       </c>
       <c r="C71" s="0">
-        <v>790.25425720214844</v>
+        <v>-1356.096321105957</v>
       </c>
       <c r="D71" s="0">
-        <v>2550.12744140625</v>
+        <v>667.942138671875</v>
       </c>
       <c r="E71" s="0">
-        <v>1531.5861206054687</v>
+        <v>-370.66378784179687</v>
       </c>
       <c r="F71" s="0">
-        <v>-5059.3343734741211</v>
+        <v>-7224.8374252319336</v>
       </c>
       <c r="G71" s="0">
-        <v>-12728.531921386719</v>
+        <v>-15179.667114257813</v>
       </c>
       <c r="H71" s="0">
-        <v>-17132.45414352417</v>
+        <v>-19691.423828125</v>
       </c>
       <c r="I71" s="0">
-        <v>-27053.767351150513</v>
+        <v>-29829.87416267395</v>
       </c>
     </row>
     <row r="72">
@@ -2410,28 +2410,28 @@
         <v>71</v>
       </c>
       <c r="B72" s="0">
-        <v>16394.646270751953</v>
+        <v>15876.094360351563</v>
       </c>
       <c r="C72" s="0">
-        <v>19718.477600097656</v>
+        <v>19123.853637695313</v>
       </c>
       <c r="D72" s="0">
-        <v>24666.470657348633</v>
+        <v>24074.733840942383</v>
       </c>
       <c r="E72" s="0">
-        <v>29160.134918212891</v>
+        <v>28474.088409423828</v>
       </c>
       <c r="F72" s="0">
-        <v>31922.149688720703</v>
+        <v>31243.984710693359</v>
       </c>
       <c r="G72" s="0">
-        <v>29057.422027587891</v>
+        <v>28438.897857666016</v>
       </c>
       <c r="H72" s="0">
-        <v>26735.991760253906</v>
+        <v>26083.992492675781</v>
       </c>
       <c r="I72" s="0">
-        <v>31959.831237792969</v>
+        <v>31015.159729003906</v>
       </c>
     </row>
     <row r="73">
@@ -2439,28 +2439,28 @@
         <v>72</v>
       </c>
       <c r="B73" s="0">
-        <v>8268.5947265625</v>
+        <v>7981.913330078125</v>
       </c>
       <c r="C73" s="0">
-        <v>13239.761764526367</v>
+        <v>13047.636657714844</v>
       </c>
       <c r="D73" s="0">
-        <v>10563.487182617188</v>
+        <v>10454.467041015625</v>
       </c>
       <c r="E73" s="0">
-        <v>8443.7111206054687</v>
+        <v>8313.3724365234375</v>
       </c>
       <c r="F73" s="0">
-        <v>10497.143005371094</v>
+        <v>10341.271728515625</v>
       </c>
       <c r="G73" s="0">
-        <v>-773.40771484375</v>
+        <v>-915.311767578125</v>
       </c>
       <c r="H73" s="0">
-        <v>-15114.532012939453</v>
+        <v>-15446.771514892578</v>
       </c>
       <c r="I73" s="0">
-        <v>-3253.8672485351562</v>
+        <v>-3632.0845336914062</v>
       </c>
     </row>
     <row r="74">
@@ -2468,28 +2468,28 @@
         <v>73</v>
       </c>
       <c r="B74" s="0">
-        <v>119627.3193359375</v>
+        <v>119878.044921875</v>
       </c>
       <c r="C74" s="0">
-        <v>72096.804565429688</v>
+        <v>72620.642456054688</v>
       </c>
       <c r="D74" s="0">
-        <v>92848.801025390625</v>
+        <v>93603.611572265625</v>
       </c>
       <c r="E74" s="0">
-        <v>115053.58569335937</v>
+        <v>115178.03100585938</v>
       </c>
       <c r="F74" s="0">
-        <v>145334.52197265625</v>
+        <v>145832.76416015625</v>
       </c>
       <c r="G74" s="0">
-        <v>122034.40063476563</v>
+        <v>121920.49047851563</v>
       </c>
       <c r="H74" s="0">
-        <v>111585.86157226562</v>
+        <v>110962.12915039063</v>
       </c>
       <c r="I74" s="0">
-        <v>133737.29418945312</v>
+        <v>133541.59887695312</v>
       </c>
     </row>
     <row r="75">
@@ -2497,28 +2497,28 @@
         <v>74</v>
       </c>
       <c r="B75" s="0">
-        <v>26432.059844970703</v>
+        <v>26524.452178955078</v>
       </c>
       <c r="C75" s="0">
-        <v>21625.806221246719</v>
+        <v>21849.974678277969</v>
       </c>
       <c r="D75" s="0">
-        <v>22116.899589538574</v>
+        <v>22082.671073913574</v>
       </c>
       <c r="E75" s="0">
-        <v>30447.75212097168</v>
+        <v>30272.62614440918</v>
       </c>
       <c r="F75" s="0">
-        <v>49637.030242919922</v>
+        <v>50007.476531982422</v>
       </c>
       <c r="G75" s="0">
-        <v>47440.800359725952</v>
+        <v>47325.135320663452</v>
       </c>
       <c r="H75" s="0">
-        <v>44194.577743530273</v>
+        <v>44254.339950561523</v>
       </c>
       <c r="I75" s="0">
-        <v>52636.57958984375</v>
+        <v>52536.330078125</v>
       </c>
     </row>
     <row r="76">
@@ -2526,28 +2526,28 @@
         <v>75</v>
       </c>
       <c r="B76" s="0">
-        <v>-1260.614027261734</v>
+        <v>-1290.6768820285797</v>
       </c>
       <c r="C76" s="0">
-        <v>-1274.2992029190063</v>
+        <v>-1297.7450742721558</v>
       </c>
       <c r="D76" s="0">
-        <v>-1534.5789310373366</v>
+        <v>-1561.8991221189499</v>
       </c>
       <c r="E76" s="0">
-        <v>-1921.625560760498</v>
+        <v>-1950.9920234680176</v>
       </c>
       <c r="F76" s="0">
-        <v>-2534.6546630859375</v>
+        <v>-2571.7445678710937</v>
       </c>
       <c r="G76" s="0">
-        <v>-2847.9828910827637</v>
+        <v>-2869.7688064575195</v>
       </c>
       <c r="H76" s="0">
-        <v>-4112.4171104431152</v>
+        <v>-4139.8437881469727</v>
       </c>
       <c r="I76" s="0">
-        <v>-6119.1981558799744</v>
+        <v>-6158.4018149375916</v>
       </c>
     </row>
     <row r="77">
@@ -2555,28 +2555,28 @@
         <v>76</v>
       </c>
       <c r="B77" s="0">
-        <v>-630.10995483398438</v>
+        <v>-4888.4944763183594</v>
       </c>
       <c r="C77" s="0">
-        <v>-3042.4533157348633</v>
+        <v>-7648.3908157348633</v>
       </c>
       <c r="D77" s="0">
-        <v>-1188.3462448120117</v>
+        <v>-6383.2351608276367</v>
       </c>
       <c r="E77" s="0">
-        <v>330.89826679229736</v>
+        <v>-4932.5200681686401</v>
       </c>
       <c r="F77" s="0">
-        <v>-1350.3672561645508</v>
+        <v>-8411.2205276489258</v>
       </c>
       <c r="G77" s="0">
-        <v>961.20326232910156</v>
+        <v>-4686.9500579833984</v>
       </c>
       <c r="H77" s="0">
-        <v>4749.3251037597656</v>
+        <v>-1613.5445251464844</v>
       </c>
       <c r="I77" s="0">
-        <v>2007.1502685546875</v>
+        <v>-4822.6495361328125</v>
       </c>
     </row>
     <row r="78">
@@ -2584,28 +2584,28 @@
         <v>77</v>
       </c>
       <c r="B78" s="0">
-        <v>31964.794998168945</v>
+        <v>31784.923843383789</v>
       </c>
       <c r="C78" s="0">
-        <v>35123.587135314941</v>
+        <v>34846.040504455566</v>
       </c>
       <c r="D78" s="0">
-        <v>36027.088928222656</v>
+        <v>35681.121826171875</v>
       </c>
       <c r="E78" s="0">
-        <v>42224.055908203125</v>
+        <v>41872.204467773438</v>
       </c>
       <c r="F78" s="0">
-        <v>54527.387756347656</v>
+        <v>54143.409851074219</v>
       </c>
       <c r="G78" s="0">
-        <v>62016.52613067627</v>
+        <v>61574.613777160645</v>
       </c>
       <c r="H78" s="0">
-        <v>62100.682159423828</v>
+        <v>61693.497467041016</v>
       </c>
       <c r="I78" s="0">
-        <v>74198.068237304688</v>
+        <v>73866.646057128906</v>
       </c>
     </row>
     <row r="79">
@@ -2613,28 +2613,28 @@
         <v>78</v>
       </c>
       <c r="B79" s="0">
-        <v>-8413.8292999267578</v>
+        <v>-8633.2783966064453</v>
       </c>
       <c r="C79" s="0">
-        <v>-4811.9851303100586</v>
+        <v>-5030.3381271362305</v>
       </c>
       <c r="D79" s="0">
-        <v>-4771.5570840835571</v>
+        <v>-4976.8528900146484</v>
       </c>
       <c r="E79" s="0">
-        <v>-3303.8250274658203</v>
+        <v>-3540.6845970153809</v>
       </c>
       <c r="F79" s="0">
-        <v>-2471.4910278320312</v>
+        <v>-2699.2314758300781</v>
       </c>
       <c r="G79" s="0">
-        <v>1590.3977355957031</v>
+        <v>1392.1532897949219</v>
       </c>
       <c r="H79" s="0">
-        <v>-983.60882568359375</v>
+        <v>-1220.7543640136719</v>
       </c>
       <c r="I79" s="0">
-        <v>-5247.1982116699219</v>
+        <v>-5611.4006652832031</v>
       </c>
     </row>
     <row r="80">
@@ -2642,28 +2642,28 @@
         <v>79</v>
       </c>
       <c r="B80" s="0">
-        <v>-13243.561004638672</v>
+        <v>-13636.864715576172</v>
       </c>
       <c r="C80" s="0">
-        <v>-13297.774505615234</v>
+        <v>-13677.123504638672</v>
       </c>
       <c r="D80" s="0">
-        <v>-12374.786865234375</v>
+        <v>-12703.4677734375</v>
       </c>
       <c r="E80" s="0">
-        <v>-12618.177505493164</v>
+        <v>-12938.20295715332</v>
       </c>
       <c r="F80" s="0">
-        <v>-17065.499336242676</v>
+        <v>-17447.468757629395</v>
       </c>
       <c r="G80" s="0">
-        <v>-19188.167938232422</v>
+        <v>-19549.056915283203</v>
       </c>
       <c r="H80" s="0">
-        <v>-18799.764910697937</v>
+        <v>-19196.980227470398</v>
       </c>
       <c r="I80" s="0">
-        <v>-20502.161933898926</v>
+        <v>-21032.171577453613</v>
       </c>
     </row>
     <row r="81">
@@ -2671,28 +2671,28 @@
         <v>80</v>
       </c>
       <c r="B81" s="0">
-        <v>-1968.2119808197021</v>
+        <v>-2102.9323635101318</v>
       </c>
       <c r="C81" s="0">
-        <v>-3032.0388107299805</v>
+        <v>-3172.7656135559082</v>
       </c>
       <c r="D81" s="0">
-        <v>-2586.3847351074219</v>
+        <v>-2709.083122253418</v>
       </c>
       <c r="E81" s="0">
-        <v>-4488.0697174072266</v>
+        <v>-4676.0999755859375</v>
       </c>
       <c r="F81" s="0">
-        <v>-6689.1400680541992</v>
+        <v>-6859.4265975952148</v>
       </c>
       <c r="G81" s="0">
-        <v>-10366.838096618652</v>
+        <v>-10535.165031433105</v>
       </c>
       <c r="H81" s="0">
-        <v>-14439.845001220703</v>
+        <v>-14640.586059570313</v>
       </c>
       <c r="I81" s="0">
-        <v>-22525.809341430664</v>
+        <v>-22851.07649230957</v>
       </c>
     </row>
     <row r="82">
@@ -2700,28 +2700,28 @@
         <v>81</v>
       </c>
       <c r="B82" s="0">
-        <v>-94150.79736328125</v>
+        <v>-102941.20166015625</v>
       </c>
       <c r="C82" s="0">
-        <v>-80467.966796875</v>
+        <v>-89200.3203125</v>
       </c>
       <c r="D82" s="0">
-        <v>-126824.90771484375</v>
+        <v>-134885.05810546875</v>
       </c>
       <c r="E82" s="0">
-        <v>-135396.20849609375</v>
+        <v>-144860.34716796875</v>
       </c>
       <c r="F82" s="0">
-        <v>-145711.81881713867</v>
+        <v>-155230.91452026367</v>
       </c>
       <c r="G82" s="0">
-        <v>-85679.08203125</v>
+        <v>-96719.7109375</v>
       </c>
       <c r="H82" s="0">
-        <v>-116126.5068359375</v>
+        <v>-128356.4775390625</v>
       </c>
       <c r="I82" s="0">
-        <v>-316743.0166015625</v>
+        <v>-327461.5595703125</v>
       </c>
     </row>
     <row r="83">
@@ -2729,28 +2729,28 @@
         <v>82</v>
       </c>
       <c r="B83" s="0">
-        <v>48474.904251098633</v>
+        <v>48261.486221313477</v>
       </c>
       <c r="C83" s="0">
-        <v>37542.91276550293</v>
+        <v>37325.811630249023</v>
       </c>
       <c r="D83" s="0">
-        <v>34981.34440612793</v>
+        <v>34710.52702331543</v>
       </c>
       <c r="E83" s="0">
-        <v>43075.575622558594</v>
+        <v>42541.546447753906</v>
       </c>
       <c r="F83" s="0">
-        <v>67552.371154785156</v>
+        <v>66851.706115722656</v>
       </c>
       <c r="G83" s="0">
-        <v>90123.065979003906</v>
+        <v>89145.994689941406</v>
       </c>
       <c r="H83" s="0">
-        <v>108349.6123046875</v>
+        <v>107521.00341796875</v>
       </c>
       <c r="I83" s="0">
-        <v>86291.56298828125</v>
+        <v>84475.86962890625</v>
       </c>
     </row>
     <row r="84">
@@ -2758,28 +2758,28 @@
         <v>83</v>
       </c>
       <c r="B84" s="0">
-        <v>-284.55794525146484</v>
+        <v>-351.56669616699219</v>
       </c>
       <c r="C84" s="0">
-        <v>-1578.3894577026367</v>
+        <v>-1641.9709701538086</v>
       </c>
       <c r="D84" s="0">
-        <v>-1437.0188446044922</v>
+        <v>-1502.8695220947266</v>
       </c>
       <c r="E84" s="0">
-        <v>63.532415390014648</v>
+        <v>-17.229776382446289</v>
       </c>
       <c r="F84" s="0">
-        <v>-105.94151306152344</v>
+        <v>-186.96994018554687</v>
       </c>
       <c r="G84" s="0">
-        <v>-796.25521755218506</v>
+        <v>-872.09094142913818</v>
       </c>
       <c r="H84" s="0">
-        <v>-662.88150787353516</v>
+        <v>-750.68697929382324</v>
       </c>
       <c r="I84" s="0">
-        <v>1771.7636032104492</v>
+        <v>1633.7429122924805</v>
       </c>
     </row>
     <row r="85">
@@ -2787,28 +2787,28 @@
         <v>84</v>
       </c>
       <c r="B85" s="0">
-        <v>-735.24375534057617</v>
+        <v>-775.2551383972168</v>
       </c>
       <c r="C85" s="0">
-        <v>-305.82797718048096</v>
+        <v>-342.04407215118408</v>
       </c>
       <c r="D85" s="0">
-        <v>67.071907043457031</v>
+        <v>30.693305969238281</v>
       </c>
       <c r="E85" s="0">
-        <v>-191.0867805480957</v>
+        <v>-235.34172439575195</v>
       </c>
       <c r="F85" s="0">
-        <v>-623.69067212939262</v>
+        <v>-674.305753916502</v>
       </c>
       <c r="G85" s="0">
-        <v>-573.64334297180176</v>
+        <v>-617.46048164367676</v>
       </c>
       <c r="H85" s="0">
-        <v>-546.05558824539185</v>
+        <v>-596.3742527961731</v>
       </c>
       <c r="I85" s="0">
-        <v>-1053.8781967163086</v>
+        <v>-1128.0632858276367</v>
       </c>
     </row>
     <row r="86">
@@ -2816,28 +2816,28 @@
         <v>85</v>
       </c>
       <c r="B86" s="0">
-        <v>21096.930786132813</v>
+        <v>20694.248413085938</v>
       </c>
       <c r="C86" s="0">
-        <v>18618.781055450439</v>
+        <v>18257.769092559814</v>
       </c>
       <c r="D86" s="0">
-        <v>20354.294254302979</v>
+        <v>19964.244724273682</v>
       </c>
       <c r="E86" s="0">
-        <v>26385.646621704102</v>
+        <v>25929.896560668945</v>
       </c>
       <c r="F86" s="0">
-        <v>34871.834312438965</v>
+        <v>34414.827659606934</v>
       </c>
       <c r="G86" s="0">
-        <v>34314.246627807617</v>
+        <v>33911.315292358398</v>
       </c>
       <c r="H86" s="0">
-        <v>38421.350387573242</v>
+        <v>38022.41374206543</v>
       </c>
       <c r="I86" s="0">
-        <v>41177.407562255859</v>
+        <v>40554.900360107422</v>
       </c>
     </row>
     <row r="87">
@@ -2845,28 +2845,28 @@
         <v>86</v>
       </c>
       <c r="B87" s="0">
-        <v>-17463.541387557983</v>
+        <v>-17280.725835800171</v>
       </c>
       <c r="C87" s="0">
-        <v>-3092.4941253662109</v>
+        <v>-3049.8554534912109</v>
       </c>
       <c r="D87" s="0">
-        <v>-7523.3121032714844</v>
+        <v>-7407.8895568847656</v>
       </c>
       <c r="E87" s="0">
-        <v>-13886.18830871582</v>
+        <v>-13717.434982299805</v>
       </c>
       <c r="F87" s="0">
-        <v>-22657.131561279297</v>
+        <v>-22574.961395263672</v>
       </c>
       <c r="G87" s="0">
-        <v>-30026.204284667969</v>
+        <v>-29965.062072753906</v>
       </c>
       <c r="H87" s="0">
-        <v>-39870.171508789063</v>
+        <v>-39759.858520507813</v>
       </c>
       <c r="I87" s="0">
-        <v>-45832.906005859375</v>
+        <v>-45658.071075439453</v>
       </c>
     </row>
     <row r="88">
@@ -2874,28 +2874,28 @@
         <v>87</v>
       </c>
       <c r="B88" s="0">
-        <v>16959.305847167969</v>
+        <v>17698.433319091797</v>
       </c>
       <c r="C88" s="0">
-        <v>22387.498550415039</v>
+        <v>23047.691360473633</v>
       </c>
       <c r="D88" s="0">
-        <v>28326.138641357422</v>
+        <v>28687.501922607422</v>
       </c>
       <c r="E88" s="0">
-        <v>30643.514526367188</v>
+        <v>31034.285888671875</v>
       </c>
       <c r="F88" s="0">
-        <v>22066.832527160645</v>
+        <v>22488.496467590332</v>
       </c>
       <c r="G88" s="0">
-        <v>26547.557723999023</v>
+        <v>26995.252059936523</v>
       </c>
       <c r="H88" s="0">
-        <v>32942.028717041016</v>
+        <v>33642.674591064453</v>
       </c>
       <c r="I88" s="0">
-        <v>42122.473114013672</v>
+        <v>42992.362152099609</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Comments to script 5 and preliminary comments to script 6
Script 5 was completley reviewed and commented. Sector 6 is commented, but there are  outputs and comments that still need to be reviewed.
</commit_message>
<xml_diff>
--- a/1-Data-Codes/2-Final_Data/deficits_allyears.xlsx
+++ b/1-Data-Codes/2-Final_Data/deficits_allyears.xlsx
@@ -411,28 +411,28 @@
         </is>
       </c>
       <c r="B2">
-        <v>-10800.4736325785</v>
+        <v>-10800.473695666</v>
       </c>
       <c r="C2">
-        <v>-11322.1676101785</v>
+        <v>-11322.1676087669</v>
       </c>
       <c r="D2">
-        <v>-11256.0183522874</v>
+        <v>-11256.0183524914</v>
       </c>
       <c r="E2">
-        <v>-11949.8204764637</v>
+        <v>-11949.8204758438</v>
       </c>
       <c r="F2">
-        <v>-12283.1880845319</v>
+        <v>-12283.1880869449</v>
       </c>
       <c r="G2">
-        <v>-15967.7151584219</v>
+        <v>-15967.7151507234</v>
       </c>
       <c r="H2">
-        <v>-13730.9881394453</v>
+        <v>-13730.9881333705</v>
       </c>
       <c r="I2">
-        <v>-13950.3202741633</v>
+        <v>-13950.3202738708</v>
       </c>
     </row>
     <row r="3">
@@ -442,28 +442,28 @@
         </is>
       </c>
       <c r="B3">
-        <v>-1021.26380364853</v>
+        <v>-1021.26380350186</v>
       </c>
       <c r="C3">
-        <v>-357.367510033641</v>
+        <v>-357.367509804059</v>
       </c>
       <c r="D3">
-        <v>-2199.8668661544</v>
+        <v>-2199.86686609595</v>
       </c>
       <c r="E3">
-        <v>-2025.2562013173</v>
+        <v>-2025.25619992192</v>
       </c>
       <c r="F3">
-        <v>-2673.2976469759</v>
+        <v>-2673.29764624567</v>
       </c>
       <c r="G3">
-        <v>-4525.52235178847</v>
+        <v>-4525.52235023726</v>
       </c>
       <c r="H3">
-        <v>-5373.08557371369</v>
+        <v>-5373.08557345821</v>
       </c>
       <c r="I3">
-        <v>-4738.83815746225</v>
+        <v>-4738.8381574727</v>
       </c>
     </row>
     <row r="4">
@@ -473,28 +473,28 @@
         </is>
       </c>
       <c r="B4">
-        <v>-2568.55447737901</v>
+        <v>-2568.5544698611</v>
       </c>
       <c r="C4">
-        <v>-2257.76853907193</v>
+        <v>-2257.76853380399</v>
       </c>
       <c r="D4">
-        <v>-4160.12674427066</v>
+        <v>-4160.12674461831</v>
       </c>
       <c r="E4">
-        <v>-524.354962351568</v>
+        <v>-524.354964745515</v>
       </c>
       <c r="F4">
-        <v>3670.25798746891</v>
+        <v>3670.25798898579</v>
       </c>
       <c r="G4">
-        <v>5363.4506391166</v>
+        <v>5363.45063824774</v>
       </c>
       <c r="H4">
-        <v>12175.0487596146</v>
+        <v>12175.0487601889</v>
       </c>
       <c r="I4">
-        <v>12183.4604133293</v>
+        <v>12183.460413574</v>
       </c>
     </row>
     <row r="5">
@@ -504,28 +504,28 @@
         </is>
       </c>
       <c r="B5">
-        <v>3318.98865960969</v>
+        <v>3318.9886580453</v>
       </c>
       <c r="C5">
-        <v>1953.33356982447</v>
+        <v>1953.33356927953</v>
       </c>
       <c r="D5">
-        <v>2115.82939205053</v>
+        <v>2115.82939208782</v>
       </c>
       <c r="E5">
-        <v>2692.65434933649</v>
+        <v>2692.65434585761</v>
       </c>
       <c r="F5">
-        <v>2420.17154278582</v>
+        <v>2420.17154695951</v>
       </c>
       <c r="G5">
-        <v>-4071.73372721739</v>
+        <v>-4071.73371932823</v>
       </c>
       <c r="H5">
-        <v>-6439.86219601029</v>
+        <v>-6439.86219514817</v>
       </c>
       <c r="I5">
-        <v>-5846.72325842613</v>
+        <v>-5846.72325859707</v>
       </c>
     </row>
     <row r="6">
@@ -535,28 +535,28 @@
         </is>
       </c>
       <c r="B6">
-        <v>-44675.5404061875</v>
+        <v>-44675.5404306067</v>
       </c>
       <c r="C6">
-        <v>-48212.3857652612</v>
+        <v>-48212.3857703173</v>
       </c>
       <c r="D6">
-        <v>-38281.9908119667</v>
+        <v>-38281.9908151637</v>
       </c>
       <c r="E6">
-        <v>-17384.0037279684</v>
+        <v>-17384.0036875898</v>
       </c>
       <c r="F6">
-        <v>-12138.5277095686</v>
+        <v>-12138.5277287733</v>
       </c>
       <c r="G6">
-        <v>8039.72865083702</v>
+        <v>8039.72862443149</v>
       </c>
       <c r="H6">
-        <v>14517.4389952059</v>
+        <v>14517.4389977807</v>
       </c>
       <c r="I6">
-        <v>-19862.9443487674</v>
+        <v>-19862.9443483406</v>
       </c>
     </row>
     <row r="7">
@@ -566,28 +566,28 @@
         </is>
       </c>
       <c r="B7">
-        <v>21166.7581494483</v>
+        <v>21166.758148437</v>
       </c>
       <c r="C7">
-        <v>19354.9553368088</v>
+        <v>19354.9553369931</v>
       </c>
       <c r="D7">
-        <v>14189.1929350276</v>
+        <v>14189.1929350397</v>
       </c>
       <c r="E7">
-        <v>10885.8691415478</v>
+        <v>10885.8691284453</v>
       </c>
       <c r="F7">
-        <v>2728.09927685366</v>
+        <v>2728.09927062804</v>
       </c>
       <c r="G7">
-        <v>-497.396093272455</v>
+        <v>-497.39609328881</v>
       </c>
       <c r="H7">
-        <v>-3149.51919022541</v>
+        <v>-3149.51919103707</v>
       </c>
       <c r="I7">
-        <v>3852.06549609239</v>
+        <v>3852.06549601233</v>
       </c>
     </row>
     <row r="8">
@@ -597,28 +597,28 @@
         </is>
       </c>
       <c r="B8">
-        <v>22163.9742211257</v>
+        <v>22163.9742227687</v>
       </c>
       <c r="C8">
-        <v>23286.9581816541</v>
+        <v>23286.9581819647</v>
       </c>
       <c r="D8">
-        <v>15596.4323505648</v>
+        <v>15596.4323498871</v>
       </c>
       <c r="E8">
-        <v>14522.7989176768</v>
+        <v>14522.7989222935</v>
       </c>
       <c r="F8">
-        <v>17630.037400248</v>
+        <v>17630.0373964915</v>
       </c>
       <c r="G8">
-        <v>13401.7843752405</v>
+        <v>13401.7843835388</v>
       </c>
       <c r="H8">
-        <v>12591.5328753879</v>
+        <v>12591.5328741562</v>
       </c>
       <c r="I8">
-        <v>22632.9635000234</v>
+        <v>22632.9635008662</v>
       </c>
     </row>
     <row r="9">
@@ -628,28 +628,28 @@
         </is>
       </c>
       <c r="B9">
-        <v>21036.4866247745</v>
+        <v>21036.4866244137</v>
       </c>
       <c r="C9">
-        <v>22943.5544751274</v>
+        <v>22943.5544746817</v>
       </c>
       <c r="D9">
-        <v>20495.7867638059</v>
+        <v>20495.7867638023</v>
       </c>
       <c r="E9">
-        <v>20504.4428032446</v>
+        <v>20504.4428013833</v>
       </c>
       <c r="F9">
-        <v>20744.9365581309</v>
+        <v>20744.9365569164</v>
       </c>
       <c r="G9">
-        <v>16223.1568695057</v>
+        <v>16223.1568717722</v>
       </c>
       <c r="H9">
-        <v>17150.3105660611</v>
+        <v>17150.3105660937</v>
       </c>
       <c r="I9">
-        <v>14864.1441053968</v>
+        <v>14864.1441054925</v>
       </c>
     </row>
     <row r="10">
@@ -659,28 +659,28 @@
         </is>
       </c>
       <c r="B10">
-        <v>-70322.7489296651</v>
+        <v>-70322.7489132378</v>
       </c>
       <c r="C10">
-        <v>-59705.4859097069</v>
+        <v>-59705.4859108031</v>
       </c>
       <c r="D10">
-        <v>-44111.4758960087</v>
+        <v>-44111.4758919774</v>
       </c>
       <c r="E10">
-        <v>-35822.3018648159</v>
+        <v>-35822.3018542619</v>
       </c>
       <c r="F10">
-        <v>-30748.3846068</v>
+        <v>-30748.3846243701</v>
       </c>
       <c r="G10">
-        <v>-10460.3517210724</v>
+        <v>-10460.3517401819</v>
       </c>
       <c r="H10">
-        <v>-15886.1235622062</v>
+        <v>-15886.1235605207</v>
       </c>
       <c r="I10">
-        <v>-40821.2560928094</v>
+        <v>-40821.2560960146</v>
       </c>
     </row>
     <row r="11">
@@ -690,28 +690,28 @@
         </is>
       </c>
       <c r="B11">
-        <v>42117.8831994219</v>
+        <v>42117.8831891364</v>
       </c>
       <c r="C11">
-        <v>40589.3300073731</v>
+        <v>40589.3300060119</v>
       </c>
       <c r="D11">
-        <v>34298.7967346801</v>
+        <v>34298.7967332512</v>
       </c>
       <c r="E11">
-        <v>35286.2287102232</v>
+        <v>35286.2286981741</v>
       </c>
       <c r="F11">
-        <v>40215.9251712546</v>
+        <v>40215.9251808712</v>
       </c>
       <c r="G11">
-        <v>36874.5729273615</v>
+        <v>36874.5729430866</v>
       </c>
       <c r="H11">
-        <v>30071.3014196087</v>
+        <v>30071.3014181761</v>
       </c>
       <c r="I11">
-        <v>23484.0507237901</v>
+        <v>23484.0507240081</v>
       </c>
     </row>
     <row r="12">
@@ -721,28 +721,28 @@
         </is>
       </c>
       <c r="B12">
-        <v>-3243.98054638016</v>
+        <v>-3243.98054461362</v>
       </c>
       <c r="C12">
-        <v>-2773.75084890365</v>
+        <v>-2773.75084893585</v>
       </c>
       <c r="D12">
-        <v>-1619.75542355136</v>
+        <v>-1619.75542363508</v>
       </c>
       <c r="E12">
-        <v>-910.881113546022</v>
+        <v>-910.881114568501</v>
       </c>
       <c r="F12">
-        <v>942.001937121316</v>
+        <v>942.001938369049</v>
       </c>
       <c r="G12">
-        <v>302.27100547503</v>
+        <v>302.271006781361</v>
       </c>
       <c r="H12">
-        <v>-806.5876761832679</v>
+        <v>-806.587676080259</v>
       </c>
       <c r="I12">
-        <v>-1005.38274975505</v>
+        <v>-1005.38274981081</v>
       </c>
     </row>
     <row r="13">
@@ -752,28 +752,28 @@
         </is>
       </c>
       <c r="B13">
-        <v>-1259.01308809166</v>
+        <v>-1259.01308871449</v>
       </c>
       <c r="C13">
-        <v>-868.23850733416</v>
+        <v>-868.2385075175</v>
       </c>
       <c r="D13">
-        <v>-1448.53494784035</v>
+        <v>-1448.53494798173</v>
       </c>
       <c r="E13">
-        <v>-1208.45817789374</v>
+        <v>-1208.45817498496</v>
       </c>
       <c r="F13">
-        <v>-1144.44866981044</v>
+        <v>-1144.44867176539</v>
       </c>
       <c r="G13">
-        <v>-2615.79940809897</v>
+        <v>-2615.79940640706</v>
       </c>
       <c r="H13">
-        <v>-520.735546661408</v>
+        <v>-520.735546416117</v>
       </c>
       <c r="I13">
-        <v>1322.51793727998</v>
+        <v>1322.51793732358</v>
       </c>
     </row>
     <row r="14">
@@ -783,28 +783,28 @@
         </is>
       </c>
       <c r="B14">
-        <v>-11989.5097680486</v>
+        <v>-11989.5097697778</v>
       </c>
       <c r="C14">
-        <v>-10196.2194128083</v>
+        <v>-10196.2194136761</v>
       </c>
       <c r="D14">
-        <v>-11201.0776307833</v>
+        <v>-11201.0776327949</v>
       </c>
       <c r="E14">
-        <v>-22391.24464076</v>
+        <v>-22391.2446466221</v>
       </c>
       <c r="F14">
-        <v>-30644.8659617965</v>
+        <v>-30644.865938785</v>
       </c>
       <c r="G14">
-        <v>-17903.0500107622</v>
+        <v>-17903.0499648176</v>
       </c>
       <c r="H14">
-        <v>-4704.66359496819</v>
+        <v>-4704.66359528656</v>
       </c>
       <c r="I14">
-        <v>5315.59858629113</v>
+        <v>5315.59858796988</v>
       </c>
     </row>
     <row r="15">
@@ -814,28 +814,28 @@
         </is>
       </c>
       <c r="B15">
-        <v>3096.54485405762</v>
+        <v>3096.54485921422</v>
       </c>
       <c r="C15">
-        <v>-1497.04072181236</v>
+        <v>-1497.04072061756</v>
       </c>
       <c r="D15">
-        <v>-7451.90581232668</v>
+        <v>-7451.90581348792</v>
       </c>
       <c r="E15">
-        <v>-6877.93849342534</v>
+        <v>-6877.93850187045</v>
       </c>
       <c r="F15">
-        <v>-13211.1961529408</v>
+        <v>-13211.1961591465</v>
       </c>
       <c r="G15">
-        <v>-23091.4902268369</v>
+        <v>-23091.4902398973</v>
       </c>
       <c r="H15">
-        <v>-25074.3211074801</v>
+        <v>-25074.321110383</v>
       </c>
       <c r="I15">
-        <v>-22428.5313331658</v>
+        <v>-22428.5313330665</v>
       </c>
     </row>
     <row r="16">
@@ -845,28 +845,28 @@
         </is>
       </c>
       <c r="B16">
-        <v>8214.28806089172</v>
+        <v>8214.288060845391</v>
       </c>
       <c r="C16">
-        <v>6666.87805120342</v>
+        <v>6666.8780517424</v>
       </c>
       <c r="D16">
-        <v>6820.46686729014</v>
+        <v>6820.46686764882</v>
       </c>
       <c r="E16">
-        <v>10848.1994598979</v>
+        <v>10848.1994568867</v>
       </c>
       <c r="F16">
-        <v>15354.3851229881</v>
+        <v>15354.3851195578</v>
       </c>
       <c r="G16">
-        <v>14775.1345435743</v>
+        <v>14775.1345517382</v>
       </c>
       <c r="H16">
-        <v>12103.4270478236</v>
+        <v>12103.4270478015</v>
       </c>
       <c r="I16">
-        <v>22364.8702058115</v>
+        <v>22364.8702058256</v>
       </c>
     </row>
     <row r="17">
@@ -876,28 +876,28 @@
         </is>
       </c>
       <c r="B17">
-        <v>6977.93478132313</v>
+        <v>6977.93478220552</v>
       </c>
       <c r="C17">
-        <v>6124.07849745028</v>
+        <v>6124.07849765151</v>
       </c>
       <c r="D17">
-        <v>6172.40051128853</v>
+        <v>6172.40051126253</v>
       </c>
       <c r="E17">
-        <v>5356.73743360883</v>
+        <v>5356.73743948554</v>
       </c>
       <c r="F17">
-        <v>1734.09689532498</v>
+        <v>1734.09689563075</v>
       </c>
       <c r="G17">
-        <v>87.8306518069088</v>
+        <v>87.8306392124708</v>
       </c>
       <c r="H17">
-        <v>1787.52801431646</v>
+        <v>1787.52801406173</v>
       </c>
       <c r="I17">
-        <v>6535.72606362898</v>
+        <v>6535.72606335968</v>
       </c>
     </row>
     <row r="18">
@@ -907,28 +907,28 @@
         </is>
       </c>
       <c r="B18">
-        <v>-22580.4450163767</v>
+        <v>-22580.445013013</v>
       </c>
       <c r="C18">
-        <v>-21951.424458649</v>
+        <v>-21951.4244589699</v>
       </c>
       <c r="D18">
-        <v>-22822.1414554152</v>
+        <v>-22822.1414553555</v>
       </c>
       <c r="E18">
-        <v>-24589.3078402206</v>
+        <v>-24589.3078387284</v>
       </c>
       <c r="F18">
-        <v>-25975.7643055443</v>
+        <v>-25975.7643021301</v>
       </c>
       <c r="G18">
-        <v>-27529.315653177</v>
+        <v>-27529.3156669623</v>
       </c>
       <c r="H18">
-        <v>-29851.1464188392</v>
+        <v>-29851.1464183178</v>
       </c>
       <c r="I18">
-        <v>-27771.741979575</v>
+        <v>-27771.741979605</v>
       </c>
     </row>
     <row r="19">
@@ -938,28 +938,28 @@
         </is>
       </c>
       <c r="B19">
-        <v>-5741.34895003378</v>
+        <v>-5741.34894728866</v>
       </c>
       <c r="C19">
-        <v>-5100.03432450602</v>
+        <v>-5100.03432539138</v>
       </c>
       <c r="D19">
-        <v>-4424.99706058023</v>
+        <v>-4424.99706035335</v>
       </c>
       <c r="E19">
-        <v>-9037.57363025493</v>
+        <v>-9037.573622926149</v>
       </c>
       <c r="F19">
-        <v>-15398.2016735726</v>
+        <v>-15398.2016688275</v>
       </c>
       <c r="G19">
-        <v>-27201.6196743341</v>
+        <v>-27201.6196787241</v>
       </c>
       <c r="H19">
-        <v>-22194.6252547514</v>
+        <v>-22194.6252544209</v>
       </c>
       <c r="I19">
-        <v>-15955.3337352386</v>
+        <v>-15955.3337351879</v>
       </c>
     </row>
     <row r="20">
@@ -969,28 +969,28 @@
         </is>
       </c>
       <c r="B20">
-        <v>-3307.19122160429</v>
+        <v>-3307.19122211655</v>
       </c>
       <c r="C20">
-        <v>-3074.9738854912</v>
+        <v>-3074.97388490157</v>
       </c>
       <c r="D20">
-        <v>-3349.75510572101</v>
+        <v>-3349.75510539707</v>
       </c>
       <c r="E20">
-        <v>-4278.61390034412</v>
+        <v>-4278.61390406625</v>
       </c>
       <c r="F20">
-        <v>-4977.00337340178</v>
+        <v>-4977.0033721765</v>
       </c>
       <c r="G20">
-        <v>-12416.7743041585</v>
+        <v>-12416.7743125312</v>
       </c>
       <c r="H20">
-        <v>-13113.8741776917</v>
+        <v>-13113.8741779493</v>
       </c>
       <c r="I20">
-        <v>-13971.941265024</v>
+        <v>-13971.9412650144</v>
       </c>
     </row>
     <row r="21">
@@ -1000,28 +1000,28 @@
         </is>
       </c>
       <c r="B21">
-        <v>-27276.7715668044</v>
+        <v>-27276.7715588064</v>
       </c>
       <c r="C21">
-        <v>-22920.2974834077</v>
+        <v>-22920.2974813137</v>
       </c>
       <c r="D21">
-        <v>-20706.4586851902</v>
+        <v>-20706.4586859615</v>
       </c>
       <c r="E21">
-        <v>-19143.1467367191</v>
+        <v>-19143.1467342845</v>
       </c>
       <c r="F21">
-        <v>-16917.0305267339</v>
+        <v>-16917.0305254039</v>
       </c>
       <c r="G21">
-        <v>-15928.8107695949</v>
+        <v>-15928.8107620745</v>
       </c>
       <c r="H21">
-        <v>-22281.1212945047</v>
+        <v>-22281.1212953375</v>
       </c>
       <c r="I21">
-        <v>-30953.0969137958</v>
+        <v>-30953.0969132465</v>
       </c>
     </row>
     <row r="22">
@@ -1031,28 +1031,28 @@
         </is>
       </c>
       <c r="B22">
-        <v>3195.00776985896</v>
+        <v>3195.00776961859</v>
       </c>
       <c r="C22">
-        <v>-688.5645252460261</v>
+        <v>-688.564529206438</v>
       </c>
       <c r="D22">
-        <v>-2891.69916868688</v>
+        <v>-2891.69916876005</v>
       </c>
       <c r="E22">
-        <v>-8043.05942239622</v>
+        <v>-8043.05942713665</v>
       </c>
       <c r="F22">
-        <v>-3883.87302147319</v>
+        <v>-3883.8730433522</v>
       </c>
       <c r="G22">
-        <v>-4741.52354721219</v>
+        <v>-4741.52358000767</v>
       </c>
       <c r="H22">
-        <v>-15825.3906951307</v>
+        <v>-15825.3906936265</v>
       </c>
       <c r="I22">
-        <v>-12554.2048963247</v>
+        <v>-12554.2048961129</v>
       </c>
     </row>
     <row r="23">
@@ -1062,28 +1062,28 @@
         </is>
       </c>
       <c r="B23">
-        <v>-83821.22534869571</v>
+        <v>-83821.22533436801</v>
       </c>
       <c r="C23">
-        <v>-90527.1466807679</v>
+        <v>-90527.1466800035</v>
       </c>
       <c r="D23">
-        <v>-89147.0263243568</v>
+        <v>-89147.0263215548</v>
       </c>
       <c r="E23">
-        <v>-94139.59888959071</v>
+        <v>-94139.5988851927</v>
       </c>
       <c r="F23">
-        <v>-108389.622829294</v>
+        <v>-108389.622832955</v>
       </c>
       <c r="G23">
-        <v>-105385.972060394</v>
+        <v>-105385.972052885</v>
       </c>
       <c r="H23">
-        <v>-124293.779086967</v>
+        <v>-124293.77909022</v>
       </c>
       <c r="I23">
-        <v>-124602.845281753</v>
+        <v>-124602.845282477</v>
       </c>
     </row>
     <row r="24">
@@ -1093,28 +1093,28 @@
         </is>
       </c>
       <c r="B24">
-        <v>-2418.90415961802</v>
+        <v>-2418.90415929402</v>
       </c>
       <c r="C24">
-        <v>-2093.81455156757</v>
+        <v>-2093.8145526205</v>
       </c>
       <c r="D24">
-        <v>-6435.61855176519</v>
+        <v>-6435.6185521936</v>
       </c>
       <c r="E24">
-        <v>-4277.23189941562</v>
+        <v>-4277.23189937633</v>
       </c>
       <c r="F24">
-        <v>-1630.44665364912</v>
+        <v>-1630.44666845394</v>
       </c>
       <c r="G24">
-        <v>5669.56019440564</v>
+        <v>5669.56019296458</v>
       </c>
       <c r="H24">
-        <v>-2000.87250055532</v>
+        <v>-2000.87250166293</v>
       </c>
       <c r="I24">
-        <v>4309.67207223829</v>
+        <v>4309.67207166061</v>
       </c>
     </row>
     <row r="25">
@@ -1124,28 +1124,28 @@
         </is>
       </c>
       <c r="B25">
-        <v>-11612.9496329272</v>
+        <v>-11612.9496315911</v>
       </c>
       <c r="C25">
-        <v>-13206.1118906946</v>
+        <v>-13206.1118901601</v>
       </c>
       <c r="D25">
-        <v>-14864.9084946922</v>
+        <v>-14864.9084946744</v>
       </c>
       <c r="E25">
-        <v>-17247.9998580827</v>
+        <v>-17247.9998548662</v>
       </c>
       <c r="F25">
-        <v>-20962.1636089389</v>
+        <v>-20962.163606977</v>
       </c>
       <c r="G25">
-        <v>-28476.5156832836</v>
+        <v>-28476.5156884656</v>
       </c>
       <c r="H25">
-        <v>-31497.5647141218</v>
+        <v>-31497.5647140325</v>
       </c>
       <c r="I25">
-        <v>-32710.294811432</v>
+        <v>-32710.2948116009</v>
       </c>
     </row>
     <row r="26">
@@ -1155,28 +1155,28 @@
         </is>
       </c>
       <c r="B26">
-        <v>-6454.55309546484</v>
+        <v>-6454.5530946215</v>
       </c>
       <c r="C26">
-        <v>-8337.54927180921</v>
+        <v>-8337.54927002586</v>
       </c>
       <c r="D26">
-        <v>-11347.8707265021</v>
+        <v>-11347.8707259444</v>
       </c>
       <c r="E26">
-        <v>-12739.372665274</v>
+        <v>-12739.3726682992</v>
       </c>
       <c r="F26">
-        <v>-13978.0337187874</v>
+        <v>-13978.0337132292</v>
       </c>
       <c r="G26">
-        <v>-10696.0964954442</v>
+        <v>-10696.0964938381</v>
       </c>
       <c r="H26">
-        <v>-10867.6633100826</v>
+        <v>-10867.6633120188</v>
       </c>
       <c r="I26">
-        <v>-13138.9631768897</v>
+        <v>-13138.9631771783</v>
       </c>
     </row>
     <row r="27">
@@ -1186,28 +1186,28 @@
         </is>
       </c>
       <c r="B27">
-        <v>-5900.77618588982</v>
+        <v>-5900.77618529036</v>
       </c>
       <c r="C27">
-        <v>-6190.90774722934</v>
+        <v>-6190.90774707734</v>
       </c>
       <c r="D27">
-        <v>-6027.53603602884</v>
+        <v>-6027.53603602476</v>
       </c>
       <c r="E27">
-        <v>-6475.44001121918</v>
+        <v>-6475.44001008384</v>
       </c>
       <c r="F27">
-        <v>-6620.72340511679</v>
+        <v>-6620.72340578983</v>
       </c>
       <c r="G27">
-        <v>-9246.94314680451</v>
+        <v>-9246.94315304358</v>
       </c>
       <c r="H27">
-        <v>-8883.5845505133</v>
+        <v>-8883.584550431309</v>
       </c>
       <c r="I27">
-        <v>-8391.70026916196</v>
+        <v>-8391.70026924129</v>
       </c>
     </row>
     <row r="28">
@@ -1217,28 +1217,28 @@
         </is>
       </c>
       <c r="B28">
-        <v>11657.6594824637</v>
+        <v>11657.6594825934</v>
       </c>
       <c r="C28">
-        <v>12125.2083318941</v>
+        <v>12125.2083321725</v>
       </c>
       <c r="D28">
-        <v>12435.0420957931</v>
+        <v>12435.0420958533</v>
       </c>
       <c r="E28">
-        <v>14178.1494302894</v>
+        <v>14178.1494290007</v>
       </c>
       <c r="F28">
-        <v>14945.3826887437</v>
+        <v>14945.3826916127</v>
       </c>
       <c r="G28">
-        <v>13536.9699427022</v>
+        <v>13536.9699413258</v>
       </c>
       <c r="H28">
-        <v>14446.4775581808</v>
+        <v>14446.4775581088</v>
       </c>
       <c r="I28">
-        <v>18749.8162251649</v>
+        <v>18749.8162252483</v>
       </c>
     </row>
     <row r="29">
@@ -1248,28 +1248,28 @@
         </is>
       </c>
       <c r="B29">
-        <v>19816.1526320978</v>
+        <v>19816.1526327028</v>
       </c>
       <c r="C29">
-        <v>20026.1056899903</v>
+        <v>20026.105689225</v>
       </c>
       <c r="D29">
-        <v>18690.3417129574</v>
+        <v>18690.3417134095</v>
       </c>
       <c r="E29">
-        <v>20797.8570726968</v>
+        <v>20797.8570746587</v>
       </c>
       <c r="F29">
-        <v>28458.542751542</v>
+        <v>28458.5427530802</v>
       </c>
       <c r="G29">
-        <v>31133.7251848731</v>
+        <v>31133.7251827017</v>
       </c>
       <c r="H29">
-        <v>31753.3900110829</v>
+        <v>31753.3900109467</v>
       </c>
       <c r="I29">
-        <v>24655.3535965645</v>
+        <v>24655.3535969228</v>
       </c>
     </row>
     <row r="30">
@@ -1279,28 +1279,28 @@
         </is>
       </c>
       <c r="B30">
-        <v>-948.287450083211</v>
+        <v>-948.2874496177331</v>
       </c>
       <c r="C30">
-        <v>-631.079497836343</v>
+        <v>-631.079497435735</v>
       </c>
       <c r="D30">
-        <v>-1336.51137594709</v>
+        <v>-1336.51137621672</v>
       </c>
       <c r="E30">
-        <v>-2656.93835639089</v>
+        <v>-2656.93835529076</v>
       </c>
       <c r="F30">
-        <v>-4317.343865435</v>
+        <v>-4317.34386624569</v>
       </c>
       <c r="G30">
-        <v>-13983.5813496154</v>
+        <v>-13983.5813478698</v>
       </c>
       <c r="H30">
-        <v>-15953.9484645698</v>
+        <v>-15953.9484645858</v>
       </c>
       <c r="I30">
-        <v>-18597.4112499114</v>
+        <v>-18597.4112499571</v>
       </c>
     </row>
     <row r="31">
@@ -1310,28 +1310,28 @@
         </is>
       </c>
       <c r="B31">
-        <v>-45716.3048391011</v>
+        <v>-45716.3048363362</v>
       </c>
       <c r="C31">
-        <v>-49106.2269011947</v>
+        <v>-49106.2269040369</v>
       </c>
       <c r="D31">
-        <v>-49300.8186407827</v>
+        <v>-49300.8186411092</v>
       </c>
       <c r="E31">
-        <v>-61422.6497200108</v>
+        <v>-61422.64972431</v>
       </c>
       <c r="F31">
-        <v>-77250.8499803897</v>
+        <v>-77250.8499708545</v>
       </c>
       <c r="G31">
-        <v>-78019.3251892898</v>
+        <v>-78019.32514875069</v>
       </c>
       <c r="H31">
-        <v>-82305.874732874</v>
+        <v>-82305.8747343677</v>
       </c>
       <c r="I31">
-        <v>-87751.0371933305</v>
+        <v>-87751.0371943536</v>
       </c>
     </row>
     <row r="32">
@@ -1341,28 +1341,28 @@
         </is>
       </c>
       <c r="B32">
-        <v>-10203.5527335171</v>
+        <v>-10203.5527330188</v>
       </c>
       <c r="C32">
-        <v>-9889.877233650681</v>
+        <v>-9889.8772345449</v>
       </c>
       <c r="D32">
-        <v>-8834.083090652381</v>
+        <v>-8834.08309089222</v>
       </c>
       <c r="E32">
-        <v>-8624.58098502053</v>
+        <v>-8624.58098300432</v>
       </c>
       <c r="F32">
-        <v>-10585.6972450306</v>
+        <v>-10585.6972450694</v>
       </c>
       <c r="G32">
-        <v>-14438.491279788</v>
+        <v>-14438.4912762016</v>
       </c>
       <c r="H32">
-        <v>-13423.2441011599</v>
+        <v>-13423.2441020507</v>
       </c>
       <c r="I32">
-        <v>-12177.9512587286</v>
+        <v>-12177.9512586435</v>
       </c>
     </row>
     <row r="33">
@@ -1372,28 +1372,28 @@
         </is>
       </c>
       <c r="B33">
-        <v>84378.5660973597</v>
+        <v>84378.566064051</v>
       </c>
       <c r="C33">
-        <v>115143.945154277</v>
+        <v>115143.945151037</v>
       </c>
       <c r="D33">
-        <v>94104.0604728203</v>
+        <v>94104.06047399181</v>
       </c>
       <c r="E33">
-        <v>73059.35009791559</v>
+        <v>73059.35015030349</v>
       </c>
       <c r="F33">
-        <v>64202.5224000024</v>
+        <v>64202.5223976539</v>
       </c>
       <c r="G33">
-        <v>85210.13392442709</v>
+        <v>85210.1340357553</v>
       </c>
       <c r="H33">
-        <v>96226.4541242108</v>
+        <v>96226.4541257431</v>
       </c>
       <c r="I33">
-        <v>98160.7650828022</v>
+        <v>98160.7650833095</v>
       </c>
     </row>
     <row r="34">
@@ -1403,28 +1403,28 @@
         </is>
       </c>
       <c r="B34">
-        <v>5903.11715242867</v>
+        <v>5903.11715309868</v>
       </c>
       <c r="C34">
-        <v>9310.94544160485</v>
+        <v>9310.945442914121</v>
       </c>
       <c r="D34">
-        <v>13625.151334357</v>
+        <v>13625.151334984</v>
       </c>
       <c r="E34">
-        <v>12843.4382395498</v>
+        <v>12843.438233563</v>
       </c>
       <c r="F34">
-        <v>14054.1019094652</v>
+        <v>14054.1019004944</v>
       </c>
       <c r="G34">
-        <v>10479.7545308229</v>
+        <v>10479.7545375487</v>
       </c>
       <c r="H34">
-        <v>8515.476659874141</v>
+        <v>8515.476659139489</v>
       </c>
       <c r="I34">
-        <v>-1069.02986816836</v>
+        <v>-1069.02986807323</v>
       </c>
     </row>
     <row r="35">
@@ -1434,28 +1434,28 @@
         </is>
       </c>
       <c r="B35">
-        <v>11.5362099104855</v>
+        <v>11.5362098007864</v>
       </c>
       <c r="C35">
-        <v>-369.164803040731</v>
+        <v>-369.16480290778</v>
       </c>
       <c r="D35">
-        <v>-619.817506789733</v>
+        <v>-619.817506802285</v>
       </c>
       <c r="E35">
-        <v>-163.150869701762</v>
+        <v>-163.150870577517</v>
       </c>
       <c r="F35">
-        <v>-10.7780600617692</v>
+        <v>-10.7780602626433</v>
       </c>
       <c r="G35">
-        <v>-1522.12788160763</v>
+        <v>-1522.12787692915</v>
       </c>
       <c r="H35">
-        <v>-1324.63047371463</v>
+        <v>-1324.63047368389</v>
       </c>
       <c r="I35">
-        <v>185.729336687082</v>
+        <v>185.72933669406</v>
       </c>
     </row>
     <row r="36">
@@ -1465,28 +1465,28 @@
         </is>
       </c>
       <c r="B36">
-        <v>-131.64280213331</v>
+        <v>-131.642780447724</v>
       </c>
       <c r="C36">
-        <v>-6683.57720737309</v>
+        <v>-6683.57720972509</v>
       </c>
       <c r="D36">
-        <v>-2376.49625062828</v>
+        <v>-2376.49625110263</v>
       </c>
       <c r="E36">
-        <v>-3285.87901161662</v>
+        <v>-3285.87900381026</v>
       </c>
       <c r="F36">
-        <v>-12151.8146925462</v>
+        <v>-12151.8146889159</v>
       </c>
       <c r="G36">
-        <v>-26463.1320786457</v>
+        <v>-26463.1320961037</v>
       </c>
       <c r="H36">
-        <v>-38131.7866400756</v>
+        <v>-38131.7866382891</v>
       </c>
       <c r="I36">
-        <v>-40292.5300389875</v>
+        <v>-40292.5300373148</v>
       </c>
     </row>
     <row r="37">
@@ -1496,28 +1496,28 @@
         </is>
       </c>
       <c r="B37">
-        <v>-7029.11775297614</v>
+        <v>-7029.11776017188</v>
       </c>
       <c r="C37">
-        <v>-5748.66385490166</v>
+        <v>-5748.66385470926</v>
       </c>
       <c r="D37">
-        <v>-5530.63955004593</v>
+        <v>-5530.63955000817</v>
       </c>
       <c r="E37">
-        <v>-7783.62703867401</v>
+        <v>-7783.62704268325</v>
       </c>
       <c r="F37">
-        <v>-8082.37438177817</v>
+        <v>-8082.37437250956</v>
       </c>
       <c r="G37">
-        <v>-19781.240411431</v>
+        <v>-19781.2404110498</v>
       </c>
       <c r="H37">
-        <v>-19799.3039280147</v>
+        <v>-19799.3039281972</v>
       </c>
       <c r="I37">
-        <v>-21107.0061881118</v>
+        <v>-21107.0061877746</v>
       </c>
     </row>
     <row r="38">
@@ -1527,28 +1527,28 @@
         </is>
       </c>
       <c r="B38">
-        <v>-7437.16030450612</v>
+        <v>-7437.16030240589</v>
       </c>
       <c r="C38">
-        <v>-10593.6371654942</v>
+        <v>-10593.6371654916</v>
       </c>
       <c r="D38">
-        <v>-14762.9927300123</v>
+        <v>-14762.9927308397</v>
       </c>
       <c r="E38">
-        <v>-15318.6159874569</v>
+        <v>-15318.6159876968</v>
       </c>
       <c r="F38">
-        <v>-17826.6348845247</v>
+        <v>-17826.6348808393</v>
       </c>
       <c r="G38">
-        <v>-18590.2742547085</v>
+        <v>-18590.2742627644</v>
       </c>
       <c r="H38">
-        <v>-14862.8569515431</v>
+        <v>-14862.856951118</v>
       </c>
       <c r="I38">
-        <v>-12022.9328472658</v>
+        <v>-12022.9328478892</v>
       </c>
     </row>
     <row r="39">
@@ -1558,28 +1558,28 @@
         </is>
       </c>
       <c r="B39">
-        <v>-81212.39785559069</v>
+        <v>-81212.3978253144</v>
       </c>
       <c r="C39">
-        <v>-82548.2804647525</v>
+        <v>-82548.28046029191</v>
       </c>
       <c r="D39">
-        <v>-87454.30516043121</v>
+        <v>-87454.3051624167</v>
       </c>
       <c r="E39">
-        <v>-94854.84626533541</v>
+        <v>-94854.8463193816</v>
       </c>
       <c r="F39">
-        <v>-98958.48723409011</v>
+        <v>-98958.4872098776</v>
       </c>
       <c r="G39">
-        <v>-108489.161874829</v>
+        <v>-108489.161894378</v>
       </c>
       <c r="H39">
-        <v>-124424.916348931</v>
+        <v>-124424.916351301</v>
       </c>
       <c r="I39">
-        <v>-107202.580301154</v>
+        <v>-107202.580301109</v>
       </c>
     </row>
     <row r="40">
@@ -1589,28 +1589,28 @@
         </is>
       </c>
       <c r="B40">
-        <v>-3907.17780627576</v>
+        <v>-3907.17780517528</v>
       </c>
       <c r="C40">
-        <v>-4082.50656510125</v>
+        <v>-4082.50656508347</v>
       </c>
       <c r="D40">
-        <v>-3946.17477322058</v>
+        <v>-3946.17477348351</v>
       </c>
       <c r="E40">
-        <v>-3769.32447400317</v>
+        <v>-3769.32447450475</v>
       </c>
       <c r="F40">
-        <v>-3841.58834459097</v>
+        <v>-3841.5883463694</v>
       </c>
       <c r="G40">
-        <v>-8091.57852702781</v>
+        <v>-8091.57853044495</v>
       </c>
       <c r="H40">
-        <v>-8756.62781444356</v>
+        <v>-8756.627813930991</v>
       </c>
       <c r="I40">
-        <v>-10487.9068030527</v>
+        <v>-10487.9068030925</v>
       </c>
     </row>
     <row r="41">
@@ -1620,28 +1620,28 @@
         </is>
       </c>
       <c r="B41">
-        <v>-15798.6477941446</v>
+        <v>-15798.6477941922</v>
       </c>
       <c r="C41">
-        <v>-18409.0429119538</v>
+        <v>-18409.0429129659</v>
       </c>
       <c r="D41">
-        <v>-21111.2624871124</v>
+        <v>-21111.2624865883</v>
       </c>
       <c r="E41">
-        <v>-21029.7322145989</v>
+        <v>-21029.7322134679</v>
       </c>
       <c r="F41">
-        <v>-23102.1298785855</v>
+        <v>-23102.12987447</v>
       </c>
       <c r="G41">
-        <v>-27332.2877239885</v>
+        <v>-27332.2877133506</v>
       </c>
       <c r="H41">
-        <v>-31728.3887759469</v>
+        <v>-31728.3887749796</v>
       </c>
       <c r="I41">
-        <v>-29425.5243979696</v>
+        <v>-29425.5243983051</v>
       </c>
     </row>
     <row r="42">
@@ -1651,28 +1651,28 @@
         </is>
       </c>
       <c r="B42">
-        <v>1586.36196372336</v>
+        <v>1586.36196318252</v>
       </c>
       <c r="C42">
-        <v>2730.70933620119</v>
+        <v>2730.70933617437</v>
       </c>
       <c r="D42">
-        <v>4367.14986579359</v>
+        <v>4367.14986589416</v>
       </c>
       <c r="E42">
-        <v>5077.51668945437</v>
+        <v>5077.51668979292</v>
       </c>
       <c r="F42">
-        <v>4977.92934520301</v>
+        <v>4977.92934483392</v>
       </c>
       <c r="G42">
-        <v>5136.12137528405</v>
+        <v>5136.12137421268</v>
       </c>
       <c r="H42">
-        <v>5410.09817512304</v>
+        <v>5410.09817514092</v>
       </c>
       <c r="I42">
-        <v>6492.94543504994</v>
+        <v>6492.94543513681</v>
       </c>
     </row>
     <row r="43">
@@ -1682,28 +1682,28 @@
         </is>
       </c>
       <c r="B43">
-        <v>13035.7216629123</v>
+        <v>13035.7216581033</v>
       </c>
       <c r="C43">
-        <v>11444.2089101543</v>
+        <v>11444.2089096018</v>
       </c>
       <c r="D43">
-        <v>10521.1057823428</v>
+        <v>10521.1057817795</v>
       </c>
       <c r="E43">
-        <v>11227.4805643214</v>
+        <v>11227.4805635268</v>
       </c>
       <c r="F43">
-        <v>11268.8259341104</v>
+        <v>11268.825938853</v>
       </c>
       <c r="G43">
-        <v>-3539.90942759771</v>
+        <v>-3539.90944700627</v>
       </c>
       <c r="H43">
-        <v>-5355.84590737556</v>
+        <v>-5355.84590659599</v>
       </c>
       <c r="I43">
-        <v>-1642.53338654996</v>
+        <v>-1642.53338659019</v>
       </c>
     </row>
     <row r="44">
@@ -1713,28 +1713,28 @@
         </is>
       </c>
       <c r="B44">
-        <v>-66166.2685933305</v>
+        <v>-66166.26858819219</v>
       </c>
       <c r="C44">
-        <v>-75549.0894097578</v>
+        <v>-75549.089407861</v>
       </c>
       <c r="D44">
-        <v>-89850.0171745535</v>
+        <v>-89850.0171728518</v>
       </c>
       <c r="E44">
-        <v>-106308.089080317</v>
+        <v>-106308.089108818</v>
       </c>
       <c r="F44">
-        <v>-126407.034344485</v>
+        <v>-126407.034336843</v>
       </c>
       <c r="G44">
-        <v>-112885.581555558</v>
+        <v>-112885.581606496</v>
       </c>
       <c r="H44">
-        <v>-99726.391838504</v>
+        <v>-99726.3918375615</v>
       </c>
       <c r="I44">
-        <v>-60075.0042072347</v>
+        <v>-60075.0042081234</v>
       </c>
     </row>
     <row r="45">
@@ -1744,28 +1744,28 @@
         </is>
       </c>
       <c r="B45">
-        <v>8086.69880312195</v>
+        <v>8086.69880281812</v>
       </c>
       <c r="C45">
-        <v>8325.631216408599</v>
+        <v>8325.63121850937</v>
       </c>
       <c r="D45">
-        <v>7642.95887295194</v>
+        <v>7642.95887316391</v>
       </c>
       <c r="E45">
-        <v>6834.48775270083</v>
+        <v>6834.48776053453</v>
       </c>
       <c r="F45">
-        <v>8122.52339895466</v>
+        <v>8122.52340014703</v>
       </c>
       <c r="G45">
-        <v>4142.90704427851</v>
+        <v>4142.90704718652</v>
       </c>
       <c r="H45">
-        <v>8758.22758417566</v>
+        <v>8758.227584097431</v>
       </c>
       <c r="I45">
-        <v>13392.8209507037</v>
+        <v>13392.8209508948</v>
       </c>
     </row>
     <row r="46">
@@ -1775,28 +1775,28 @@
         </is>
       </c>
       <c r="B46">
-        <v>-5381.74426159938</v>
+        <v>-5381.74426180349</v>
       </c>
       <c r="C46">
-        <v>-5564.17927475519</v>
+        <v>-5564.17927470403</v>
       </c>
       <c r="D46">
-        <v>-5193.34425744555</v>
+        <v>-5193.34425743259</v>
       </c>
       <c r="E46">
-        <v>-5629.31293770404</v>
+        <v>-5629.31293755285</v>
       </c>
       <c r="F46">
-        <v>-5078.22405562163</v>
+        <v>-5078.22405539386</v>
       </c>
       <c r="G46">
-        <v>-6263.30060285535</v>
+        <v>-6263.30060301562</v>
       </c>
       <c r="H46">
-        <v>-8352.813258314411</v>
+        <v>-8352.81325847882</v>
       </c>
       <c r="I46">
-        <v>-8405.04716571467</v>
+        <v>-8405.047165683651</v>
       </c>
     </row>
     <row r="47">
@@ -1806,28 +1806,28 @@
         </is>
       </c>
       <c r="B47">
-        <v>-224.938367458082</v>
+        <v>-224.938364493926</v>
       </c>
       <c r="C47">
-        <v>4031.7046393696</v>
+        <v>4031.70464101597</v>
       </c>
       <c r="D47">
-        <v>4202.16498648526</v>
+        <v>4202.16498857327</v>
       </c>
       <c r="E47">
-        <v>5284.82555655093</v>
+        <v>5284.82555127103</v>
       </c>
       <c r="F47">
-        <v>3206.6487788858</v>
+        <v>3206.64877863971</v>
       </c>
       <c r="G47">
-        <v>-10182.4770199789</v>
+        <v>-10182.477059827</v>
       </c>
       <c r="H47">
-        <v>-12643.0683671486</v>
+        <v>-12643.0683660328</v>
       </c>
       <c r="I47">
-        <v>-18405.2439748659</v>
+        <v>-18405.2439744046</v>
       </c>
     </row>
     <row r="48">
@@ -1837,28 +1837,28 @@
         </is>
       </c>
       <c r="B48">
-        <v>6250.11357584637</v>
+        <v>6250.11358253814</v>
       </c>
       <c r="C48">
-        <v>5390.20938921782</v>
+        <v>5390.20939034289</v>
       </c>
       <c r="D48">
-        <v>4693.54327411719</v>
+        <v>4693.54327340297</v>
       </c>
       <c r="E48">
-        <v>5447.89203061533</v>
+        <v>5447.89203663843</v>
       </c>
       <c r="F48">
-        <v>-11335.7949196635</v>
+        <v>-11335.7949240058</v>
       </c>
       <c r="G48">
-        <v>-11399.2941573268</v>
+        <v>-11399.2941396701</v>
       </c>
       <c r="H48">
-        <v>-3550.363395238</v>
+        <v>-3550.36339531247</v>
       </c>
       <c r="I48">
-        <v>19727.6114418352</v>
+        <v>19727.6114416215</v>
       </c>
     </row>
     <row r="49">
@@ -1868,28 +1868,28 @@
         </is>
       </c>
       <c r="B49">
-        <v>-8185.96102720221</v>
+        <v>-8185.96102721216</v>
       </c>
       <c r="C49">
-        <v>-8717.653149029989</v>
+        <v>-8717.65314773405</v>
       </c>
       <c r="D49">
-        <v>-9471.245785608109</v>
+        <v>-9471.24578538777</v>
       </c>
       <c r="E49">
-        <v>-10660.3735929286</v>
+        <v>-10660.3735935551</v>
       </c>
       <c r="F49">
-        <v>-11348.2093342997</v>
+        <v>-11348.2093322216</v>
       </c>
       <c r="G49">
-        <v>-15980.4779899275</v>
+        <v>-15980.4779873653</v>
       </c>
       <c r="H49">
-        <v>-16225.8443657604</v>
+        <v>-16225.8443660896</v>
       </c>
       <c r="I49">
-        <v>-15719.0974530428</v>
+        <v>-15719.0974529357</v>
       </c>
     </row>
     <row r="50">
@@ -1899,28 +1899,28 @@
         </is>
       </c>
       <c r="B50">
-        <v>-11179.5932764128</v>
+        <v>-11179.5932671153</v>
       </c>
       <c r="C50">
-        <v>-11661.9310308311</v>
+        <v>-11661.9310337159</v>
       </c>
       <c r="D50">
-        <v>-12803.8515147452</v>
+        <v>-12803.8515142287</v>
       </c>
       <c r="E50">
-        <v>-15628.8686765462</v>
+        <v>-15628.8686787476</v>
       </c>
       <c r="F50">
-        <v>-17261.5079293598</v>
+        <v>-17261.5079391008</v>
       </c>
       <c r="G50">
-        <v>-21689.4565968929</v>
+        <v>-21689.4566061637</v>
       </c>
       <c r="H50">
-        <v>-26815.405455162</v>
+        <v>-26815.4054569718</v>
       </c>
       <c r="I50">
-        <v>-26349.6522287463</v>
+        <v>-26349.6522285565</v>
       </c>
     </row>
     <row r="51">
@@ -1930,28 +1930,28 @@
         </is>
       </c>
       <c r="B51">
-        <v>-2432.33739539635</v>
+        <v>-2432.3373951874</v>
       </c>
       <c r="C51">
-        <v>-2521.07112887004</v>
+        <v>-2521.07112898121</v>
       </c>
       <c r="D51">
-        <v>-2141.34035296054</v>
+        <v>-2141.34035293602</v>
       </c>
       <c r="E51">
-        <v>-2837.94658997511</v>
+        <v>-2837.9465891287</v>
       </c>
       <c r="F51">
-        <v>-3564.02695200379</v>
+        <v>-3564.02695163519</v>
       </c>
       <c r="G51">
-        <v>-4617.06878101445</v>
+        <v>-4617.06878096793</v>
       </c>
       <c r="H51">
-        <v>-3948.86512146676</v>
+        <v>-3948.86512161156</v>
       </c>
       <c r="I51">
-        <v>-3229.13434760957</v>
+        <v>-3229.13434772534</v>
       </c>
     </row>
     <row r="52">
@@ -1961,28 +1961,28 @@
         </is>
       </c>
       <c r="B52">
-        <v>4235.82359563213</v>
+        <v>4235.82359562776</v>
       </c>
       <c r="C52">
-        <v>2804.79307428506</v>
+        <v>2804.79307429182</v>
       </c>
       <c r="D52">
-        <v>-5802.58444396636</v>
+        <v>-5802.58444396601</v>
       </c>
       <c r="E52">
-        <v>-10756.5052856709</v>
+        <v>-10756.5052855713</v>
       </c>
       <c r="F52">
-        <v>-13568.0890155817</v>
+        <v>-13568.0890155749</v>
       </c>
       <c r="G52">
-        <v>-9633.72409418136</v>
+        <v>-9633.72409420127</v>
       </c>
       <c r="H52">
         <v>-6457.63042023878</v>
       </c>
       <c r="I52">
-        <v>-15536.2704990663</v>
+        <v>-15536.2704990666</v>
       </c>
     </row>
     <row r="53">
@@ -1992,28 +1992,28 @@
         </is>
       </c>
       <c r="B53">
-        <v>2677.40314245289</v>
+        <v>2677.40314245071</v>
       </c>
       <c r="C53">
-        <v>3486.22034112292</v>
+        <v>3486.22034112269</v>
       </c>
       <c r="D53">
-        <v>7702.08556904597</v>
+        <v>7702.08556904594</v>
       </c>
       <c r="E53">
-        <v>6447.28312014319</v>
+        <v>6447.28312017782</v>
       </c>
       <c r="F53">
-        <v>7878.3046284047</v>
+        <v>7878.30462840994</v>
       </c>
       <c r="G53">
-        <v>9582.82448979081</v>
+        <v>9582.82448979553</v>
       </c>
       <c r="H53">
-        <v>15187.0877705896</v>
+        <v>15187.0877705898</v>
       </c>
       <c r="I53">
-        <v>19452.3166044172</v>
+        <v>19452.3166044191</v>
       </c>
     </row>
     <row r="54">
@@ -2023,28 +2023,28 @@
         </is>
       </c>
       <c r="B54">
-        <v>12393.5984256832</v>
+        <v>12393.598425691</v>
       </c>
       <c r="C54">
-        <v>14444.6730196482</v>
+        <v>14444.6730196584</v>
       </c>
       <c r="D54">
-        <v>18868.168275273</v>
+        <v>18868.1682752741</v>
       </c>
       <c r="E54">
-        <v>22897.8812312551</v>
+        <v>22897.8812313441</v>
       </c>
       <c r="F54">
-        <v>25331.1388832935</v>
+        <v>25331.1388833189</v>
       </c>
       <c r="G54">
-        <v>22493.5745439959</v>
+        <v>22493.5745439212</v>
       </c>
       <c r="H54">
-        <v>24797.5385536151</v>
+        <v>24797.5385536249</v>
       </c>
       <c r="I54">
-        <v>28572.7992535761</v>
+        <v>28572.7992535734</v>
       </c>
     </row>
     <row r="55">
@@ -2054,28 +2054,28 @@
         </is>
       </c>
       <c r="B55">
-        <v>-247.146889724265</v>
+        <v>-247.146889724133</v>
       </c>
       <c r="C55">
-        <v>-974.913685308331</v>
+        <v>-974.913685308293</v>
       </c>
       <c r="D55">
-        <v>-1098.67406068498</v>
+        <v>-1098.67406068473</v>
       </c>
       <c r="E55">
-        <v>-1660.8921096444</v>
+        <v>-1660.89210964418</v>
       </c>
       <c r="F55">
-        <v>-2322.61226132867</v>
+        <v>-2322.61226132789</v>
       </c>
       <c r="G55">
-        <v>-3563.74215260273</v>
+        <v>-3563.74215260198</v>
       </c>
       <c r="H55">
-        <v>-2727.33810144115</v>
+        <v>-2727.33810144105</v>
       </c>
       <c r="I55">
-        <v>-7071.71595096161</v>
+        <v>-7071.71595096154</v>
       </c>
     </row>
     <row r="56">
@@ -2085,28 +2085,28 @@
         </is>
       </c>
       <c r="B56">
-        <v>-4787.98010659097</v>
+        <v>-4787.9801065933</v>
       </c>
       <c r="C56">
-        <v>-1097.00583505312</v>
+        <v>-1097.0058350572</v>
       </c>
       <c r="D56">
-        <v>12769.8374142506</v>
+        <v>12769.8374142525</v>
       </c>
       <c r="E56">
-        <v>20662.8798040296</v>
+        <v>20662.8798040341</v>
       </c>
       <c r="F56">
-        <v>31223.634314091</v>
+        <v>31223.6343140875</v>
       </c>
       <c r="G56">
-        <v>38349.574559464</v>
+        <v>38349.5745594524</v>
       </c>
       <c r="H56">
-        <v>39481.0161702124</v>
+        <v>39481.0161702111</v>
       </c>
       <c r="I56">
-        <v>31045.0069420728</v>
+        <v>31045.006942073</v>
       </c>
     </row>
     <row r="57">
@@ -2116,28 +2116,28 @@
         </is>
       </c>
       <c r="B57">
-        <v>47081.0996724455</v>
+        <v>47081.0996724584</v>
       </c>
       <c r="C57">
-        <v>43163.6631799014</v>
+        <v>43163.6631798719</v>
       </c>
       <c r="D57">
-        <v>36761.2518898125</v>
+        <v>36761.2518897671</v>
       </c>
       <c r="E57">
-        <v>36864.1964021111</v>
+        <v>36864.1964019971</v>
       </c>
       <c r="F57">
-        <v>46651.8913360064</v>
+        <v>46651.8913356735</v>
       </c>
       <c r="G57">
-        <v>43854.6647068671</v>
+        <v>43854.6647080557</v>
       </c>
       <c r="H57">
-        <v>36943.067522508</v>
+        <v>36943.0675225216</v>
       </c>
       <c r="I57">
-        <v>33079.5472154798</v>
+        <v>33079.5472154759</v>
       </c>
     </row>
     <row r="58">
@@ -2147,28 +2147,28 @@
         </is>
       </c>
       <c r="B58">
-        <v>41589.1132512288</v>
+        <v>41589.1132512239</v>
       </c>
       <c r="C58">
-        <v>41308.1412145824</v>
+        <v>41308.1412145668</v>
       </c>
       <c r="D58">
-        <v>53174.3400078685</v>
+        <v>53174.3400078697</v>
       </c>
       <c r="E58">
-        <v>59466.173187818</v>
+        <v>59466.1731876652</v>
       </c>
       <c r="F58">
-        <v>82604.621630758</v>
+        <v>82604.6216308304</v>
       </c>
       <c r="G58">
-        <v>165077.977901055</v>
+        <v>165077.977901132</v>
       </c>
       <c r="H58">
-        <v>258369.25786178</v>
+        <v>258369.257861747</v>
       </c>
       <c r="I58">
-        <v>369380.034165449</v>
+        <v>369380.034165444</v>
       </c>
     </row>
     <row r="59">
@@ -2178,28 +2178,28 @@
         </is>
       </c>
       <c r="B59">
-        <v>-1840.687839635</v>
+        <v>-1840.6878396349</v>
       </c>
       <c r="C59">
-        <v>-1824.30944423803</v>
+        <v>-1824.30944423794</v>
       </c>
       <c r="D59">
-        <v>-2075.48867173515</v>
+        <v>-2075.48867173533</v>
       </c>
       <c r="E59">
-        <v>-2385.37428107436</v>
+        <v>-2385.37428107317</v>
       </c>
       <c r="F59">
-        <v>-2674.93823739255</v>
+        <v>-2674.93823739296</v>
       </c>
       <c r="G59">
-        <v>-2759.48486593339</v>
+        <v>-2759.4848659138</v>
       </c>
       <c r="H59">
-        <v>-3194.46010505614</v>
+        <v>-3194.46010505615</v>
       </c>
       <c r="I59">
-        <v>-4329.49482069111</v>
+        <v>-4329.49482069142</v>
       </c>
     </row>
     <row r="60">
@@ -2209,28 +2209,28 @@
         </is>
       </c>
       <c r="B60">
-        <v>-1300.60932191445</v>
+        <v>-1300.60932192004</v>
       </c>
       <c r="C60">
-        <v>-989.449612808897</v>
+        <v>-989.449612806467</v>
       </c>
       <c r="D60">
-        <v>-1099.04634596853</v>
+        <v>-1099.04634597119</v>
       </c>
       <c r="E60">
-        <v>-1499.71338441934</v>
+        <v>-1499.71338439416</v>
       </c>
       <c r="F60">
-        <v>739.336289015504</v>
+        <v>739.336288995102</v>
       </c>
       <c r="G60">
-        <v>4645.77425984912</v>
+        <v>4645.77425986024</v>
       </c>
       <c r="H60">
-        <v>5671.13715303936</v>
+        <v>5671.13715304012</v>
       </c>
       <c r="I60">
-        <v>8927.50241559516</v>
+        <v>8927.502415595831</v>
       </c>
     </row>
     <row r="61">
@@ -2240,28 +2240,28 @@
         </is>
       </c>
       <c r="B61">
-        <v>65255.6733103798</v>
+        <v>65255.6733103693</v>
       </c>
       <c r="C61">
-        <v>90025.5847572577</v>
+        <v>90025.584757217</v>
       </c>
       <c r="D61">
-        <v>140655.700964129</v>
+        <v>140655.700964154</v>
       </c>
       <c r="E61">
-        <v>161166.855215476</v>
+        <v>161166.855215609</v>
       </c>
       <c r="F61">
-        <v>207259.217059232</v>
+        <v>207259.217059341</v>
       </c>
       <c r="G61">
-        <v>221146.93886649</v>
+        <v>221146.93886573</v>
       </c>
       <c r="H61">
-        <v>236087.202755908</v>
+        <v>236087.20275596</v>
       </c>
       <c r="I61">
-        <v>315605.235569815</v>
+        <v>315605.235569801</v>
       </c>
     </row>
     <row r="62">
@@ -2271,28 +2271,28 @@
         </is>
       </c>
       <c r="B62">
-        <v>10629.0095145682</v>
+        <v>10629.0095145709</v>
       </c>
       <c r="C62">
-        <v>11461.3157544385</v>
+        <v>11461.3157544384</v>
       </c>
       <c r="D62">
-        <v>11175.5210216588</v>
+        <v>11175.521021655</v>
       </c>
       <c r="E62">
-        <v>14489.7427183509</v>
+        <v>14489.742718338</v>
       </c>
       <c r="F62">
-        <v>13889.2579806193</v>
+        <v>13889.2579806543</v>
       </c>
       <c r="G62">
-        <v>14047.616505798</v>
+        <v>14047.6165057798</v>
       </c>
       <c r="H62">
-        <v>10347.7079939127</v>
+        <v>10347.7079939195</v>
       </c>
       <c r="I62">
-        <v>10029.7299577417</v>
+        <v>10029.7299577397</v>
       </c>
     </row>
     <row r="63">
@@ -2302,28 +2302,28 @@
         </is>
       </c>
       <c r="B63">
-        <v>-30896.0547897468</v>
+        <v>-30896.0547897451</v>
       </c>
       <c r="C63">
-        <v>-29046.9966724697</v>
+        <v>-29046.9966724779</v>
       </c>
       <c r="D63">
-        <v>-29903.9831727931</v>
+        <v>-29903.9831727973</v>
       </c>
       <c r="E63">
-        <v>-40020.9622574495</v>
+        <v>-40020.9622574856</v>
       </c>
       <c r="F63">
-        <v>-60176.6524883674</v>
+        <v>-60176.6524884361</v>
       </c>
       <c r="G63">
-        <v>-74472.04169913</v>
+        <v>-74472.0416991223</v>
       </c>
       <c r="H63">
-        <v>-90009.4542715315</v>
+        <v>-90009.4542715354</v>
       </c>
       <c r="I63">
-        <v>-109586.02140908</v>
+        <v>-109586.021409079</v>
       </c>
     </row>
     <row r="64">
@@ -2333,28 +2333,28 @@
         </is>
       </c>
       <c r="B64">
-        <v>-563.354121202931</v>
+        <v>-563.354121202833</v>
       </c>
       <c r="C64">
-        <v>-1390.3302962083</v>
+        <v>-1390.33029620861</v>
       </c>
       <c r="D64">
-        <v>-865.877432104828</v>
+        <v>-865.877432104959</v>
       </c>
       <c r="E64">
-        <v>-1651.94889181854</v>
+        <v>-1651.94889181672</v>
       </c>
       <c r="F64">
-        <v>-2291.11977788826</v>
+        <v>-2291.11977788739</v>
       </c>
       <c r="G64">
-        <v>-1865.90580030462</v>
+        <v>-1865.9058003036</v>
       </c>
       <c r="H64">
         <v>-2111.713025625</v>
       </c>
       <c r="I64">
-        <v>-2739.39215551551</v>
+        <v>-2739.39215551545</v>
       </c>
     </row>
     <row r="65">
@@ -2364,28 +2364,28 @@
         </is>
       </c>
       <c r="B65">
-        <v>12812.5741465204</v>
+        <v>12812.5741465268</v>
       </c>
       <c r="C65">
-        <v>12950.8768973649</v>
+        <v>12950.8768973612</v>
       </c>
       <c r="D65">
-        <v>13948.3696362342</v>
+        <v>13948.3696362357</v>
       </c>
       <c r="E65">
-        <v>13208.8157166355</v>
+        <v>13208.8157166142</v>
       </c>
       <c r="F65">
-        <v>14820.6940273318</v>
+        <v>14820.6940273643</v>
       </c>
       <c r="G65">
-        <v>11084.9972861014</v>
+        <v>11084.9972861128</v>
       </c>
       <c r="H65">
-        <v>13294.8947977119</v>
+        <v>13294.8947977085</v>
       </c>
       <c r="I65">
-        <v>15923.6243921363</v>
+        <v>15923.6243921365</v>
       </c>
     </row>
     <row r="66">
@@ -2395,28 +2395,28 @@
         </is>
       </c>
       <c r="B66">
-        <v>19851.4659158977</v>
+        <v>19851.4659158276</v>
       </c>
       <c r="C66">
-        <v>20749.3379910562</v>
+        <v>20749.3379910737</v>
       </c>
       <c r="D66">
-        <v>25496.9720088505</v>
+        <v>25496.9720088533</v>
       </c>
       <c r="E66">
-        <v>23528.4597398663</v>
+        <v>23528.4597396777</v>
       </c>
       <c r="F66">
-        <v>16568.932980454</v>
+        <v>16568.9329805071</v>
       </c>
       <c r="G66">
-        <v>-391.573186894741</v>
+        <v>-391.573186783913</v>
       </c>
       <c r="H66">
-        <v>-6578.61050119999</v>
+        <v>-6578.61050119626</v>
       </c>
       <c r="I66">
-        <v>-19314.9406363204</v>
+        <v>-19314.9406363264</v>
       </c>
     </row>
     <row r="67">
@@ -2426,28 +2426,28 @@
         </is>
       </c>
       <c r="B67">
-        <v>6322.84232828699</v>
+        <v>6322.84232817616</v>
       </c>
       <c r="C67">
-        <v>-1445.80200588001</v>
+        <v>-1445.80200595009</v>
       </c>
       <c r="D67">
-        <v>-6548.33148451313</v>
+        <v>-6548.33148450707</v>
       </c>
       <c r="E67">
-        <v>-2222.47133686856</v>
+        <v>-2222.47133740453</v>
       </c>
       <c r="F67">
-        <v>-9290.6344619145</v>
+        <v>-9290.63446175571</v>
       </c>
       <c r="G67">
-        <v>-21864.6503900327</v>
+        <v>-21864.6503906059</v>
       </c>
       <c r="H67">
-        <v>-17181.7430700336</v>
+        <v>-17181.7430700113</v>
       </c>
       <c r="I67">
-        <v>-20805.6390047661</v>
+        <v>-20805.6390047559</v>
       </c>
     </row>
     <row r="68">
@@ -2457,28 +2457,28 @@
         </is>
       </c>
       <c r="B68">
-        <v>-20161.6049038538</v>
+        <v>-20161.6049038586</v>
       </c>
       <c r="C68">
-        <v>-21166.4102905889</v>
+        <v>-21166.4102905997</v>
       </c>
       <c r="D68">
-        <v>-25016.7663048289</v>
+        <v>-25016.7663048191</v>
       </c>
       <c r="E68">
-        <v>-29224.668702218</v>
+        <v>-29224.6687021783</v>
       </c>
       <c r="F68">
-        <v>-29781.3154713624</v>
+        <v>-29781.3154713424</v>
       </c>
       <c r="G68">
-        <v>-29823.0348719319</v>
+        <v>-29823.0348719544</v>
       </c>
       <c r="H68">
-        <v>-35604.810413061</v>
+        <v>-35604.810413066</v>
       </c>
       <c r="I68">
-        <v>-45764.4819778267</v>
+        <v>-45764.4819778248</v>
       </c>
     </row>
     <row r="69">
@@ -2488,28 +2488,28 @@
         </is>
       </c>
       <c r="B69">
-        <v>-2227.66456793942</v>
+        <v>-2227.66456793917</v>
       </c>
       <c r="C69">
-        <v>-1462.77532137665</v>
+        <v>-1462.77532138224</v>
       </c>
       <c r="D69">
-        <v>-1339.45439657451</v>
+        <v>-1339.45439657696</v>
       </c>
       <c r="E69">
-        <v>-2524.52776668069</v>
+        <v>-2524.52776666519</v>
       </c>
       <c r="F69">
-        <v>-2137.13328865108</v>
+        <v>-2137.13328865016</v>
       </c>
       <c r="G69">
-        <v>-523.948113685041</v>
+        <v>-523.948113695111</v>
       </c>
       <c r="H69">
-        <v>1776.75081116293</v>
+        <v>1776.75081116159</v>
       </c>
       <c r="I69">
-        <v>4189.55569534333</v>
+        <v>4189.55569534314</v>
       </c>
     </row>
     <row r="70">
@@ -2519,28 +2519,28 @@
         </is>
       </c>
       <c r="B70">
-        <v>16920.6872261739</v>
+        <v>16920.6872261761</v>
       </c>
       <c r="C70">
-        <v>14472.367275541</v>
+        <v>14472.3672755431</v>
       </c>
       <c r="D70">
-        <v>14086.5944290917</v>
+        <v>14086.5944290932</v>
       </c>
       <c r="E70">
-        <v>18265.2961759965</v>
+        <v>18265.2961759877</v>
       </c>
       <c r="F70">
-        <v>13250.1836327506</v>
+        <v>13250.183632734</v>
       </c>
       <c r="G70">
-        <v>13275.6798228322</v>
+        <v>13275.6798228503</v>
       </c>
       <c r="H70">
-        <v>21192.1228054767</v>
+        <v>21192.1228054772</v>
       </c>
       <c r="I70">
-        <v>19971.1996902551</v>
+        <v>19971.1996902544</v>
       </c>
     </row>
     <row r="71">
@@ -2550,28 +2550,28 @@
         </is>
       </c>
       <c r="B71">
-        <v>-223.616976635998</v>
+        <v>-223.616976634659</v>
       </c>
       <c r="C71">
-        <v>-46.1643091026763</v>
+        <v>-46.1643091005226</v>
       </c>
       <c r="D71">
-        <v>1758.98822081268</v>
+        <v>1758.98822081128</v>
       </c>
       <c r="E71">
-        <v>510.999207365143</v>
+        <v>510.999207336039</v>
       </c>
       <c r="F71">
-        <v>-6893.75272189505</v>
+        <v>-6893.752721899</v>
       </c>
       <c r="G71">
-        <v>-14843.0347021023</v>
+        <v>-14843.0347021309</v>
       </c>
       <c r="H71">
-        <v>-20519.3766427871</v>
+        <v>-20519.3766427886</v>
       </c>
       <c r="I71">
-        <v>-30985.126216575</v>
+        <v>-30985.1262165761</v>
       </c>
     </row>
     <row r="72">
@@ -2581,28 +2581,28 @@
         </is>
       </c>
       <c r="B72">
-        <v>14665.6455136589</v>
+        <v>14665.6455137366</v>
       </c>
       <c r="C72">
-        <v>17647.6548895656</v>
+        <v>17647.6548895775</v>
       </c>
       <c r="D72">
-        <v>22516.8188807429</v>
+        <v>22516.8188807474</v>
       </c>
       <c r="E72">
-        <v>26224.1431839087</v>
+        <v>26224.1431842668</v>
       </c>
       <c r="F72">
-        <v>28824.4532063945</v>
+        <v>28824.4532065106</v>
       </c>
       <c r="G72">
-        <v>24985.9210731449</v>
+        <v>24985.9210737253</v>
       </c>
       <c r="H72">
-        <v>22973.0631077361</v>
+        <v>22973.0631076839</v>
       </c>
       <c r="I72">
-        <v>26442.7265501955</v>
+        <v>26442.7265501835</v>
       </c>
     </row>
     <row r="73">
@@ -2612,28 +2612,28 @@
         </is>
       </c>
       <c r="B73">
-        <v>12543.4066985519</v>
+        <v>12543.4066985852</v>
       </c>
       <c r="C73">
-        <v>18631.4380780652</v>
+        <v>18631.4380781304</v>
       </c>
       <c r="D73">
-        <v>14727.0555082808</v>
+        <v>14727.0555082773</v>
       </c>
       <c r="E73">
-        <v>15008.5881107556</v>
+        <v>15008.5881106681</v>
       </c>
       <c r="F73">
-        <v>17311.793978233</v>
+        <v>17311.7939783403</v>
       </c>
       <c r="G73">
-        <v>10714.9798560925</v>
+        <v>10714.9798558983</v>
       </c>
       <c r="H73">
-        <v>2845.94621236562</v>
+        <v>2845.94621237447</v>
       </c>
       <c r="I73">
-        <v>13288.6198694329</v>
+        <v>13288.6198694376</v>
       </c>
     </row>
     <row r="74">
@@ -2643,28 +2643,28 @@
         </is>
       </c>
       <c r="B74">
-        <v>125615.23335022</v>
+        <v>125615.233350125</v>
       </c>
       <c r="C74">
-        <v>78239.80591070961</v>
+        <v>78239.8059106333</v>
       </c>
       <c r="D74">
-        <v>98068.0927114708</v>
+        <v>98068.092711488</v>
       </c>
       <c r="E74">
-        <v>122024.828973858</v>
+        <v>122024.828973948</v>
       </c>
       <c r="F74">
-        <v>152842.745257105</v>
+        <v>152842.745257142</v>
       </c>
       <c r="G74">
-        <v>133875.24217172</v>
+        <v>133875.242171267</v>
       </c>
       <c r="H74">
-        <v>127178.51728749</v>
+        <v>127178.517287478</v>
       </c>
       <c r="I74">
-        <v>152112.213911923</v>
+        <v>152112.213911915</v>
       </c>
     </row>
     <row r="75">
@@ -2674,28 +2674,28 @@
         </is>
       </c>
       <c r="B75">
-        <v>27456.2669450073</v>
+        <v>27456.2669450453</v>
       </c>
       <c r="C75">
-        <v>22667.0299575249</v>
+        <v>22667.0299575302</v>
       </c>
       <c r="D75">
-        <v>23322.3367796387</v>
+        <v>23322.3367796351</v>
       </c>
       <c r="E75">
-        <v>32670.9895361193</v>
+        <v>32670.989536228</v>
       </c>
       <c r="F75">
-        <v>51449.7472289251</v>
+        <v>51449.7472286626</v>
       </c>
       <c r="G75">
-        <v>50519.2291230184</v>
+        <v>50519.2291233664</v>
       </c>
       <c r="H75">
-        <v>48444.4624481441</v>
+        <v>48444.4624481226</v>
       </c>
       <c r="I75">
-        <v>57627.5829206309</v>
+        <v>57627.5829206378</v>
       </c>
     </row>
     <row r="76">
@@ -2705,28 +2705,28 @@
         </is>
       </c>
       <c r="B76">
-        <v>-1102.10423728233</v>
+        <v>-1102.10423728223</v>
       </c>
       <c r="C76">
-        <v>-1162.62237912506</v>
+        <v>-1162.62237912495</v>
       </c>
       <c r="D76">
-        <v>-1226.21348669187</v>
+        <v>-1226.21348669183</v>
       </c>
       <c r="E76">
-        <v>-1610.80516828072</v>
+        <v>-1610.80516827957</v>
       </c>
       <c r="F76">
-        <v>-2310.093117375</v>
+        <v>-2310.09311737548</v>
       </c>
       <c r="G76">
-        <v>-2667.7714993458</v>
+        <v>-2667.771499345</v>
       </c>
       <c r="H76">
-        <v>-3863.94059071407</v>
+        <v>-3863.94059071408</v>
       </c>
       <c r="I76">
-        <v>-6048.00636409905</v>
+        <v>-6048.00636409906</v>
       </c>
     </row>
     <row r="77">
@@ -2736,28 +2736,28 @@
         </is>
       </c>
       <c r="B77">
-        <v>-5436.4379689287</v>
+        <v>-5436.43796892235</v>
       </c>
       <c r="C77">
-        <v>-7580.18716138778</v>
+        <v>-7580.18716139616</v>
       </c>
       <c r="D77">
-        <v>-6108.17152396617</v>
+        <v>-6108.17152396151</v>
       </c>
       <c r="E77">
-        <v>-5083.20598016068</v>
+        <v>-5083.20598013379</v>
       </c>
       <c r="F77">
-        <v>-7482.65747183504</v>
+        <v>-7482.6574718305</v>
       </c>
       <c r="G77">
-        <v>-7529.96246133308</v>
+        <v>-7529.96246143785</v>
       </c>
       <c r="H77">
-        <v>-3010.73218164584</v>
+        <v>-3010.73218164677</v>
       </c>
       <c r="I77">
-        <v>-5982.20254458733</v>
+        <v>-5982.2025445878</v>
       </c>
     </row>
     <row r="78">
@@ -2767,28 +2767,28 @@
         </is>
       </c>
       <c r="B78">
-        <v>32916.7034697617</v>
+        <v>32916.7034697885</v>
       </c>
       <c r="C78">
-        <v>36433.539662351</v>
+        <v>36433.5396624068</v>
       </c>
       <c r="D78">
-        <v>36895.8852282256</v>
+        <v>36895.885228219</v>
       </c>
       <c r="E78">
-        <v>44492.1005319507</v>
+        <v>44492.1005319444</v>
       </c>
       <c r="F78">
-        <v>57168.1788685965</v>
+        <v>57168.1788686609</v>
       </c>
       <c r="G78">
-        <v>65546.62268253919</v>
+        <v>65546.622683002</v>
       </c>
       <c r="H78">
-        <v>67307.2338317604</v>
+        <v>67307.2338317986</v>
       </c>
       <c r="I78">
-        <v>78696.7965867732</v>
+        <v>78696.796586775</v>
       </c>
     </row>
     <row r="79">
@@ -2798,28 +2798,28 @@
         </is>
       </c>
       <c r="B79">
-        <v>-8184.22570059127</v>
+        <v>-8184.22570059002</v>
       </c>
       <c r="C79">
-        <v>-4769.81111583548</v>
+        <v>-4769.81111583333</v>
       </c>
       <c r="D79">
-        <v>-4907.00761382178</v>
+        <v>-4907.00761381977</v>
       </c>
       <c r="E79">
-        <v>-3188.31395072038</v>
+        <v>-3188.31395073543</v>
       </c>
       <c r="F79">
-        <v>-2692.49343084505</v>
+        <v>-2692.49343084604</v>
       </c>
       <c r="G79">
-        <v>1929.17977456542</v>
+        <v>1929.17977453742</v>
       </c>
       <c r="H79">
-        <v>243.370926615804</v>
+        <v>243.370926622149</v>
       </c>
       <c r="I79">
-        <v>-2980.46297209567</v>
+        <v>-2980.46297209614</v>
       </c>
     </row>
     <row r="80">
@@ -2829,28 +2829,28 @@
         </is>
       </c>
       <c r="B80">
-        <v>-12877.6083940335</v>
+        <v>-12877.6083940347</v>
       </c>
       <c r="C80">
-        <v>-12848.4856834466</v>
+        <v>-12848.48568345</v>
       </c>
       <c r="D80">
-        <v>-11841.6575256269</v>
+        <v>-11841.657525629</v>
       </c>
       <c r="E80">
-        <v>-12080.9532340072</v>
+        <v>-12080.9532340241</v>
       </c>
       <c r="F80">
-        <v>-16369.4905738029</v>
+        <v>-16369.4905738024</v>
       </c>
       <c r="G80">
-        <v>-18067.0588095797</v>
+        <v>-18067.0588095788</v>
       </c>
       <c r="H80">
-        <v>-17861.1456420189</v>
+        <v>-17861.1456420188</v>
       </c>
       <c r="I80">
-        <v>-19370.2199648631</v>
+        <v>-19370.2199648638</v>
       </c>
     </row>
     <row r="81">
@@ -2860,90 +2860,90 @@
         </is>
       </c>
       <c r="B81">
-        <v>-1331.64243223005</v>
+        <v>-1331.64243223032</v>
       </c>
       <c r="C81">
-        <v>-2312.46205016723</v>
+        <v>-2312.46205016777</v>
       </c>
       <c r="D81">
-        <v>-1762.76078777027</v>
+        <v>-1762.76078776996</v>
       </c>
       <c r="E81">
-        <v>-3188.03910828203</v>
+        <v>-3188.03910827519</v>
       </c>
       <c r="F81">
-        <v>-4537.77443087886</v>
+        <v>-4537.77443088054</v>
       </c>
       <c r="G81">
-        <v>-7528.27979898078</v>
+        <v>-7528.27979898099</v>
       </c>
       <c r="H81">
-        <v>-11486.7258029294</v>
+        <v>-11486.7258029295</v>
       </c>
       <c r="I81">
-        <v>-19104.9277530621</v>
+        <v>-19104.9277530619</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>RoW</t>
+          <t>RUS</t>
         </is>
       </c>
       <c r="B82">
-        <v>-125965.683554221</v>
+        <v>-321726.725162348</v>
       </c>
       <c r="C82">
-        <v>-113897.631707981</v>
+        <v>-451601.567495175</v>
       </c>
       <c r="D82">
-        <v>-153616.879115666</v>
+        <v>-415419.147334554</v>
       </c>
       <c r="E82">
-        <v>-173884.614482151</v>
+        <v>-450380.587163282</v>
       </c>
       <c r="F82">
-        <v>-193907.439660194</v>
+        <v>-414576.248250888</v>
       </c>
       <c r="G82">
-        <v>-162444.18391821</v>
+        <v>-302357.376138546</v>
       </c>
       <c r="H82">
-        <v>-215097.52628898</v>
+        <v>-300100.602247038</v>
       </c>
       <c r="I82">
-        <v>-410890.745456232</v>
+        <v>-536650.46769176</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>RUS</t>
+          <t>RoW</t>
         </is>
       </c>
       <c r="B83">
-        <v>41260.9695453023</v>
+        <v>237022.011154175</v>
       </c>
       <c r="C83">
-        <v>29005.1355109714</v>
+        <v>366709.071298569</v>
       </c>
       <c r="D83">
-        <v>26772.0544480871</v>
+        <v>288574.322666958</v>
       </c>
       <c r="E83">
-        <v>31223.0604493372</v>
+        <v>307719.033133934</v>
       </c>
       <c r="F83">
-        <v>48839.5499184734</v>
+        <v>269508.358506965</v>
       </c>
       <c r="G83">
-        <v>66026.4561025811</v>
+        <v>205939.648319507</v>
       </c>
       <c r="H83">
-        <v>83374.84931722999</v>
+        <v>168377.925275066</v>
       </c>
       <c r="I83">
-        <v>51984.9227493014</v>
+        <v>177744.644984811</v>
       </c>
     </row>
     <row r="84">
@@ -2953,28 +2953,28 @@
         </is>
       </c>
       <c r="B84">
-        <v>-327.96348554572</v>
+        <v>-327.963485545975</v>
       </c>
       <c r="C84">
-        <v>-1616.8438288932</v>
+        <v>-1616.84382889213</v>
       </c>
       <c r="D84">
-        <v>-1382.33609727874</v>
+        <v>-1382.33609727861</v>
       </c>
       <c r="E84">
-        <v>160.819588701852</v>
+        <v>160.819588703962</v>
       </c>
       <c r="F84">
-        <v>838.5417963742281</v>
+        <v>838.5417963756111</v>
       </c>
       <c r="G84">
-        <v>-35.6953850588941</v>
+        <v>-35.6953850578172</v>
       </c>
       <c r="H84">
-        <v>775.038672307473</v>
+        <v>775.038672307575</v>
       </c>
       <c r="I84">
-        <v>3629.09872021136</v>
+        <v>3629.09872021151</v>
       </c>
     </row>
     <row r="85">
@@ -2984,25 +2984,25 @@
         </is>
       </c>
       <c r="B85">
-        <v>-677.854281630467</v>
+        <v>-677.854281630259</v>
       </c>
       <c r="C85">
-        <v>-225.340786711569</v>
+        <v>-225.340786711653</v>
       </c>
       <c r="D85">
-        <v>155.939042583906</v>
+        <v>155.939042584099</v>
       </c>
       <c r="E85">
-        <v>-157.851517624583</v>
+        <v>-157.85151762697</v>
       </c>
       <c r="F85">
-        <v>-686.9811511888749</v>
+        <v>-686.981151189275</v>
       </c>
       <c r="G85">
-        <v>-655.8782887806919</v>
+        <v>-655.878288784221</v>
       </c>
       <c r="H85">
-        <v>-637.113856217084</v>
+        <v>-637.113856217244</v>
       </c>
       <c r="I85">
         <v>-1203.07001530484</v>
@@ -3015,28 +3015,28 @@
         </is>
       </c>
       <c r="B86">
-        <v>21240.4591154397</v>
+        <v>21240.4591154712</v>
       </c>
       <c r="C86">
-        <v>18407.4201392966</v>
+        <v>18407.4201393162</v>
       </c>
       <c r="D86">
-        <v>19806.6621241461</v>
+        <v>19806.6621241422</v>
       </c>
       <c r="E86">
-        <v>25621.2091034458</v>
+        <v>25621.2091035479</v>
       </c>
       <c r="F86">
-        <v>33555.8627385982</v>
+        <v>33555.8627386147</v>
       </c>
       <c r="G86">
-        <v>32564.9647015723</v>
+        <v>32564.9647015208</v>
       </c>
       <c r="H86">
-        <v>36484.0851467327</v>
+        <v>36484.0851467305</v>
       </c>
       <c r="I86">
-        <v>39666.419698214</v>
+        <v>39666.4196982075</v>
       </c>
     </row>
     <row r="87">
@@ -3046,25 +3046,25 @@
         </is>
       </c>
       <c r="B87">
-        <v>-16554.5081145806</v>
+        <v>-16554.5081145818</v>
       </c>
       <c r="C87">
-        <v>-1706.62467165228</v>
+        <v>-1706.62467165225</v>
       </c>
       <c r="D87">
         <v>-5020.73166934738</v>
       </c>
       <c r="E87">
-        <v>-10922.7661418628</v>
+        <v>-10922.7661418627</v>
       </c>
       <c r="F87">
-        <v>-18742.599989623</v>
+        <v>-18742.5999896232</v>
       </c>
       <c r="G87">
-        <v>-24715.2794116543</v>
+        <v>-24715.2794116584</v>
       </c>
       <c r="H87">
-        <v>-32320.8189388822</v>
+        <v>-32320.8189388824</v>
       </c>
       <c r="I87">
         <v>-36977.4332951847</v>
@@ -3077,28 +3077,28 @@
         </is>
       </c>
       <c r="B88">
-        <v>18175.3607078209</v>
+        <v>18175.3607078736</v>
       </c>
       <c r="C88">
-        <v>23574.6432190149</v>
+        <v>23574.6432190071</v>
       </c>
       <c r="D88">
-        <v>29464.5307658725</v>
+        <v>29464.5307658833</v>
       </c>
       <c r="E88">
-        <v>31320.9036645172</v>
+        <v>31320.9036645154</v>
       </c>
       <c r="F88">
-        <v>22840.5707477869</v>
+        <v>22840.5707477284</v>
       </c>
       <c r="G88">
-        <v>27311.3258965101</v>
+        <v>27311.3258964509</v>
       </c>
       <c r="H88">
-        <v>34207.761445692</v>
+        <v>34207.7614457022</v>
       </c>
       <c r="I88">
-        <v>43498.8484091661</v>
+        <v>43498.8484091691</v>
       </c>
     </row>
   </sheetData>

</xml_diff>